<commit_message>
update tai lieu sau khi chinh sua mot vai sai xot
</commit_message>
<xml_diff>
--- a/2015/201512/10_DOCUMENT/13_DETAIL_DESIGN/Bao cao KH moi theo nhan vien/CRMF3010_ Khach hang moi theo nhan vien.xlsx
+++ b/2015/201512/10_DOCUMENT/13_DETAIL_DESIGN/Bao cao KH moi theo nhan vien/CRMF3010_ Khach hang moi theo nhan vien.xlsx
@@ -2384,24 +2384,25 @@
 @@FromEmployeeID @@ToEmployeeID Biến môi trường</t>
   </si>
   <si>
-    <t>Menu [Báo cáo] -&gt; MenuItem[Báo cáo Thống kê] 
+    <t>Nhận tham số @FormID từ màn hình Báo cáo biểu đồ CRMF3000 để mởi màn hình CRMF3010</t>
+  </si>
+  <si>
+    <t>Đổ nguồn DropdownCheckList đơn vị</t>
+  </si>
+  <si>
+    <t>Đổ nguồn DropdownCheckList chọn kỳ</t>
+  </si>
+  <si>
+    <t>Thực thi @SQL0003, @SQL0004 phụ thuộc vào @DivisionID của câu @SQL0001</t>
+  </si>
+  <si>
+    <t>@FormID</t>
+  </si>
+  <si>
+    <t>Menu [Báo cáo]
+ -&gt; MenuItem[Báo cáo biểu đồ_CRMF3000] 
 -&gt; Click vào Link Báo cáo KH mới theo nhân viên 
 -&gt;Pop [Báo cáo khách hàng mới theo nhân viên_CRMF3010]</t>
-  </si>
-  <si>
-    <t>Nhận tham số @FormID từ màn hình Báo cáo biểu đồ CRMF3000 để mởi màn hình CRMF3010</t>
-  </si>
-  <si>
-    <t>Đổ nguồn DropdownCheckList đơn vị</t>
-  </si>
-  <si>
-    <t>Đổ nguồn DropdownCheckList chọn kỳ</t>
-  </si>
-  <si>
-    <t>Thực thi @SQL0003, @SQL0004 phụ thuộc vào @DivisionID của câu @SQL0001</t>
-  </si>
-  <si>
-    <t>@FormID</t>
   </si>
 </sst>
 </file>
@@ -3269,9 +3270,27 @@
     <xf numFmtId="0" fontId="11" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="26" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="26" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="26" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3317,23 +3336,8 @@
     <xf numFmtId="0" fontId="31" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="26" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="26" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="26" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -3374,9 +3378,6 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3438,6 +3439,18 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3445,18 +3458,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -4407,65 +4408,65 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="27" customHeight="1">
-      <c r="A1" s="142"/>
-      <c r="B1" s="142"/>
-      <c r="C1" s="144" t="s">
+      <c r="A1" s="148"/>
+      <c r="B1" s="148"/>
+      <c r="C1" s="150" t="s">
         <v>155</v>
       </c>
-      <c r="D1" s="145"/>
-      <c r="E1" s="145"/>
-      <c r="F1" s="146"/>
-      <c r="G1" s="143" t="s">
+      <c r="D1" s="151"/>
+      <c r="E1" s="151"/>
+      <c r="F1" s="152"/>
+      <c r="G1" s="149" t="s">
         <v>151</v>
       </c>
-      <c r="H1" s="143"/>
-      <c r="I1" s="143" t="s">
+      <c r="H1" s="149"/>
+      <c r="I1" s="149" t="s">
         <v>152</v>
       </c>
-      <c r="J1" s="143"/>
+      <c r="J1" s="149"/>
     </row>
     <row r="2" spans="1:18" ht="23.25" customHeight="1">
-      <c r="A2" s="142"/>
-      <c r="B2" s="142"/>
-      <c r="C2" s="147"/>
-      <c r="D2" s="148"/>
-      <c r="E2" s="148"/>
-      <c r="F2" s="149"/>
-      <c r="G2" s="143" t="s">
+      <c r="A2" s="148"/>
+      <c r="B2" s="148"/>
+      <c r="C2" s="153"/>
+      <c r="D2" s="154"/>
+      <c r="E2" s="154"/>
+      <c r="F2" s="155"/>
+      <c r="G2" s="149" t="s">
         <v>153</v>
       </c>
-      <c r="H2" s="143"/>
-      <c r="I2" s="143"/>
-      <c r="J2" s="143"/>
+      <c r="H2" s="149"/>
+      <c r="I2" s="149"/>
+      <c r="J2" s="149"/>
     </row>
     <row r="3" spans="1:18" ht="12.75" customHeight="1">
-      <c r="A3" s="142"/>
-      <c r="B3" s="142"/>
-      <c r="C3" s="150"/>
-      <c r="D3" s="151"/>
-      <c r="E3" s="151"/>
-      <c r="F3" s="152"/>
-      <c r="G3" s="139" t="s">
+      <c r="A3" s="148"/>
+      <c r="B3" s="148"/>
+      <c r="C3" s="156"/>
+      <c r="D3" s="157"/>
+      <c r="E3" s="157"/>
+      <c r="F3" s="158"/>
+      <c r="G3" s="145" t="s">
         <v>154</v>
       </c>
-      <c r="H3" s="140"/>
-      <c r="I3" s="139"/>
-      <c r="J3" s="140"/>
+      <c r="H3" s="146"/>
+      <c r="I3" s="145"/>
+      <c r="J3" s="146"/>
     </row>
     <row r="4" spans="1:18">
       <c r="H4" s="117"/>
     </row>
     <row r="13" spans="1:18" ht="30">
-      <c r="A13" s="141"/>
-      <c r="B13" s="141"/>
-      <c r="C13" s="141"/>
-      <c r="D13" s="141"/>
-      <c r="E13" s="141"/>
-      <c r="F13" s="141"/>
-      <c r="G13" s="141"/>
-      <c r="H13" s="141"/>
-      <c r="I13" s="141"/>
-      <c r="J13" s="141"/>
+      <c r="A13" s="147"/>
+      <c r="B13" s="147"/>
+      <c r="C13" s="147"/>
+      <c r="D13" s="147"/>
+      <c r="E13" s="147"/>
+      <c r="F13" s="147"/>
+      <c r="G13" s="147"/>
+      <c r="H13" s="147"/>
+      <c r="I13" s="147"/>
+      <c r="J13" s="147"/>
       <c r="K13" s="118"/>
       <c r="L13" s="118"/>
       <c r="M13" s="118"/>
@@ -4476,56 +4477,56 @@
       <c r="R13" s="118"/>
     </row>
     <row r="14" spans="1:18" ht="26.25">
-      <c r="B14" s="137"/>
-      <c r="C14" s="137"/>
-      <c r="D14" s="137"/>
-      <c r="E14" s="137"/>
-      <c r="F14" s="137"/>
-      <c r="G14" s="137"/>
-      <c r="H14" s="137"/>
-      <c r="I14" s="137"/>
-      <c r="J14" s="137"/>
-      <c r="K14" s="137"/>
-      <c r="L14" s="137"/>
-      <c r="M14" s="137"/>
-      <c r="N14" s="137"/>
-      <c r="O14" s="137"/>
-      <c r="P14" s="137"/>
-      <c r="Q14" s="137"/>
-      <c r="R14" s="137"/>
+      <c r="B14" s="141"/>
+      <c r="C14" s="141"/>
+      <c r="D14" s="141"/>
+      <c r="E14" s="141"/>
+      <c r="F14" s="141"/>
+      <c r="G14" s="141"/>
+      <c r="H14" s="141"/>
+      <c r="I14" s="141"/>
+      <c r="J14" s="141"/>
+      <c r="K14" s="141"/>
+      <c r="L14" s="141"/>
+      <c r="M14" s="141"/>
+      <c r="N14" s="141"/>
+      <c r="O14" s="141"/>
+      <c r="P14" s="141"/>
+      <c r="Q14" s="141"/>
+      <c r="R14" s="141"/>
     </row>
     <row r="15" spans="1:18" ht="26.25">
-      <c r="B15" s="137"/>
-      <c r="C15" s="137"/>
-      <c r="D15" s="137"/>
-      <c r="E15" s="137"/>
-      <c r="F15" s="137"/>
-      <c r="G15" s="137"/>
-      <c r="H15" s="137"/>
-      <c r="I15" s="137"/>
-      <c r="J15" s="137"/>
-      <c r="K15" s="137"/>
-      <c r="L15" s="137"/>
-      <c r="M15" s="137"/>
-      <c r="N15" s="137"/>
-      <c r="O15" s="137"/>
-      <c r="P15" s="137"/>
-      <c r="Q15" s="137"/>
-      <c r="R15" s="137"/>
+      <c r="B15" s="141"/>
+      <c r="C15" s="141"/>
+      <c r="D15" s="141"/>
+      <c r="E15" s="141"/>
+      <c r="F15" s="141"/>
+      <c r="G15" s="141"/>
+      <c r="H15" s="141"/>
+      <c r="I15" s="141"/>
+      <c r="J15" s="141"/>
+      <c r="K15" s="141"/>
+      <c r="L15" s="141"/>
+      <c r="M15" s="141"/>
+      <c r="N15" s="141"/>
+      <c r="O15" s="141"/>
+      <c r="P15" s="141"/>
+      <c r="Q15" s="141"/>
+      <c r="R15" s="141"/>
     </row>
     <row r="16" spans="1:18" ht="26.25">
-      <c r="A16" s="138" t="s">
+      <c r="A16" s="144" t="s">
         <v>157</v>
       </c>
-      <c r="B16" s="138"/>
-      <c r="C16" s="138"/>
-      <c r="D16" s="138"/>
-      <c r="E16" s="138"/>
-      <c r="F16" s="138"/>
-      <c r="G16" s="138"/>
-      <c r="H16" s="138"/>
-      <c r="I16" s="138"/>
-      <c r="J16" s="138"/>
+      <c r="B16" s="144"/>
+      <c r="C16" s="144"/>
+      <c r="D16" s="144"/>
+      <c r="E16" s="144"/>
+      <c r="F16" s="144"/>
+      <c r="G16" s="144"/>
+      <c r="H16" s="144"/>
+      <c r="I16" s="144"/>
+      <c r="J16" s="144"/>
       <c r="K16" s="119"/>
       <c r="L16" s="119"/>
       <c r="M16" s="119"/>
@@ -4536,384 +4537,384 @@
       <c r="R16" s="119"/>
     </row>
     <row r="17" spans="1:195" ht="14.1" customHeight="1">
-      <c r="B17" s="137"/>
-      <c r="C17" s="137"/>
-      <c r="D17" s="137"/>
-      <c r="E17" s="137"/>
-      <c r="F17" s="137"/>
-      <c r="G17" s="137"/>
-      <c r="H17" s="137"/>
-      <c r="I17" s="137"/>
-      <c r="J17" s="137"/>
-      <c r="K17" s="137"/>
-      <c r="L17" s="137"/>
-      <c r="M17" s="137"/>
-      <c r="N17" s="137"/>
-      <c r="O17" s="137"/>
-      <c r="P17" s="137"/>
-      <c r="Q17" s="137"/>
-      <c r="R17" s="137"/>
+      <c r="B17" s="141"/>
+      <c r="C17" s="141"/>
+      <c r="D17" s="141"/>
+      <c r="E17" s="141"/>
+      <c r="F17" s="141"/>
+      <c r="G17" s="141"/>
+      <c r="H17" s="141"/>
+      <c r="I17" s="141"/>
+      <c r="J17" s="141"/>
+      <c r="K17" s="141"/>
+      <c r="L17" s="141"/>
+      <c r="M17" s="141"/>
+      <c r="N17" s="141"/>
+      <c r="O17" s="141"/>
+      <c r="P17" s="141"/>
+      <c r="Q17" s="141"/>
+      <c r="R17" s="141"/>
     </row>
     <row r="18" spans="1:195" ht="26.25">
-      <c r="B18" s="137"/>
-      <c r="C18" s="137"/>
-      <c r="D18" s="137"/>
-      <c r="E18" s="137"/>
-      <c r="F18" s="137"/>
-      <c r="G18" s="137"/>
-      <c r="H18" s="137"/>
-      <c r="I18" s="137"/>
-      <c r="J18" s="137"/>
-      <c r="K18" s="137"/>
-      <c r="L18" s="137"/>
-      <c r="M18" s="137"/>
-      <c r="N18" s="137"/>
-      <c r="O18" s="137"/>
-      <c r="P18" s="137"/>
-      <c r="Q18" s="137"/>
-      <c r="R18" s="137"/>
+      <c r="B18" s="141"/>
+      <c r="C18" s="141"/>
+      <c r="D18" s="141"/>
+      <c r="E18" s="141"/>
+      <c r="F18" s="141"/>
+      <c r="G18" s="141"/>
+      <c r="H18" s="141"/>
+      <c r="I18" s="141"/>
+      <c r="J18" s="141"/>
+      <c r="K18" s="141"/>
+      <c r="L18" s="141"/>
+      <c r="M18" s="141"/>
+      <c r="N18" s="141"/>
+      <c r="O18" s="141"/>
+      <c r="P18" s="141"/>
+      <c r="Q18" s="141"/>
+      <c r="R18" s="141"/>
     </row>
     <row r="19" spans="1:195" ht="23.25">
-      <c r="B19" s="154"/>
-      <c r="C19" s="154"/>
-      <c r="D19" s="154"/>
-      <c r="E19" s="154"/>
-      <c r="F19" s="154"/>
-      <c r="G19" s="154"/>
-      <c r="H19" s="154"/>
-      <c r="I19" s="154"/>
-      <c r="J19" s="154"/>
-      <c r="K19" s="154"/>
-      <c r="L19" s="154"/>
-      <c r="M19" s="154"/>
-      <c r="N19" s="154"/>
-      <c r="O19" s="154"/>
-      <c r="P19" s="154"/>
-      <c r="Q19" s="154"/>
-      <c r="R19" s="154"/>
+      <c r="B19" s="143"/>
+      <c r="C19" s="143"/>
+      <c r="D19" s="143"/>
+      <c r="E19" s="143"/>
+      <c r="F19" s="143"/>
+      <c r="G19" s="143"/>
+      <c r="H19" s="143"/>
+      <c r="I19" s="143"/>
+      <c r="J19" s="143"/>
+      <c r="K19" s="143"/>
+      <c r="L19" s="143"/>
+      <c r="M19" s="143"/>
+      <c r="N19" s="143"/>
+      <c r="O19" s="143"/>
+      <c r="P19" s="143"/>
+      <c r="Q19" s="143"/>
+      <c r="R19" s="143"/>
     </row>
     <row r="20" spans="1:195" ht="26.25">
-      <c r="B20" s="137"/>
-      <c r="C20" s="137"/>
-      <c r="D20" s="137"/>
-      <c r="E20" s="137"/>
-      <c r="F20" s="137"/>
-      <c r="G20" s="137"/>
-      <c r="H20" s="137"/>
-      <c r="I20" s="137"/>
-      <c r="J20" s="137"/>
-      <c r="K20" s="137"/>
-      <c r="L20" s="137"/>
-      <c r="M20" s="137"/>
-      <c r="N20" s="137"/>
-      <c r="O20" s="137"/>
-      <c r="P20" s="137"/>
-      <c r="Q20" s="137"/>
-      <c r="R20" s="137"/>
+      <c r="B20" s="141"/>
+      <c r="C20" s="141"/>
+      <c r="D20" s="141"/>
+      <c r="E20" s="141"/>
+      <c r="F20" s="141"/>
+      <c r="G20" s="141"/>
+      <c r="H20" s="141"/>
+      <c r="I20" s="141"/>
+      <c r="J20" s="141"/>
+      <c r="K20" s="141"/>
+      <c r="L20" s="141"/>
+      <c r="M20" s="141"/>
+      <c r="N20" s="141"/>
+      <c r="O20" s="141"/>
+      <c r="P20" s="141"/>
+      <c r="Q20" s="141"/>
+      <c r="R20" s="141"/>
     </row>
     <row r="21" spans="1:195" ht="26.25">
-      <c r="B21" s="137"/>
-      <c r="C21" s="137"/>
-      <c r="D21" s="137"/>
-      <c r="E21" s="137"/>
-      <c r="F21" s="137"/>
-      <c r="G21" s="137"/>
-      <c r="H21" s="137"/>
-      <c r="I21" s="137"/>
-      <c r="J21" s="137"/>
-      <c r="K21" s="137"/>
-      <c r="L21" s="137"/>
-      <c r="M21" s="137"/>
-      <c r="N21" s="137"/>
-      <c r="O21" s="137"/>
-      <c r="P21" s="137"/>
-      <c r="Q21" s="137"/>
-      <c r="R21" s="137"/>
+      <c r="B21" s="141"/>
+      <c r="C21" s="141"/>
+      <c r="D21" s="141"/>
+      <c r="E21" s="141"/>
+      <c r="F21" s="141"/>
+      <c r="G21" s="141"/>
+      <c r="H21" s="141"/>
+      <c r="I21" s="141"/>
+      <c r="J21" s="141"/>
+      <c r="K21" s="141"/>
+      <c r="L21" s="141"/>
+      <c r="M21" s="141"/>
+      <c r="N21" s="141"/>
+      <c r="O21" s="141"/>
+      <c r="P21" s="141"/>
+      <c r="Q21" s="141"/>
+      <c r="R21" s="141"/>
     </row>
     <row r="22" spans="1:195" ht="25.5">
-      <c r="B22" s="153"/>
-      <c r="C22" s="153"/>
-      <c r="D22" s="153"/>
-      <c r="E22" s="153"/>
-      <c r="F22" s="153"/>
-      <c r="G22" s="153"/>
-      <c r="H22" s="153"/>
-      <c r="I22" s="153"/>
-      <c r="J22" s="153"/>
-      <c r="K22" s="153"/>
-      <c r="L22" s="153"/>
-      <c r="M22" s="153"/>
-      <c r="N22" s="153"/>
-      <c r="O22" s="153"/>
-      <c r="P22" s="153"/>
-      <c r="Q22" s="153"/>
-      <c r="R22" s="153"/>
+      <c r="B22" s="142"/>
+      <c r="C22" s="142"/>
+      <c r="D22" s="142"/>
+      <c r="E22" s="142"/>
+      <c r="F22" s="142"/>
+      <c r="G22" s="142"/>
+      <c r="H22" s="142"/>
+      <c r="I22" s="142"/>
+      <c r="J22" s="142"/>
+      <c r="K22" s="142"/>
+      <c r="L22" s="142"/>
+      <c r="M22" s="142"/>
+      <c r="N22" s="142"/>
+      <c r="O22" s="142"/>
+      <c r="P22" s="142"/>
+      <c r="Q22" s="142"/>
+      <c r="R22" s="142"/>
     </row>
     <row r="23" spans="1:195" ht="25.5">
-      <c r="B23" s="153"/>
-      <c r="C23" s="153"/>
-      <c r="D23" s="153"/>
-      <c r="E23" s="153"/>
-      <c r="F23" s="153"/>
-      <c r="G23" s="153"/>
-      <c r="H23" s="153"/>
-      <c r="I23" s="153"/>
-      <c r="J23" s="153"/>
-      <c r="K23" s="153"/>
-      <c r="L23" s="153"/>
-      <c r="M23" s="153"/>
-      <c r="N23" s="153"/>
-      <c r="O23" s="153"/>
-      <c r="P23" s="153"/>
-      <c r="Q23" s="153"/>
-      <c r="R23" s="153"/>
+      <c r="B23" s="142"/>
+      <c r="C23" s="142"/>
+      <c r="D23" s="142"/>
+      <c r="E23" s="142"/>
+      <c r="F23" s="142"/>
+      <c r="G23" s="142"/>
+      <c r="H23" s="142"/>
+      <c r="I23" s="142"/>
+      <c r="J23" s="142"/>
+      <c r="K23" s="142"/>
+      <c r="L23" s="142"/>
+      <c r="M23" s="142"/>
+      <c r="N23" s="142"/>
+      <c r="O23" s="142"/>
+      <c r="P23" s="142"/>
+      <c r="Q23" s="142"/>
+      <c r="R23" s="142"/>
     </row>
     <row r="25" spans="1:195" ht="11.25" customHeight="1"/>
     <row r="26" spans="1:195" ht="18">
-      <c r="B26" s="155"/>
-      <c r="C26" s="155"/>
-      <c r="D26" s="155"/>
-      <c r="E26" s="155"/>
-      <c r="F26" s="155"/>
-      <c r="G26" s="155"/>
-      <c r="H26" s="155"/>
-      <c r="I26" s="155"/>
-      <c r="J26" s="155"/>
-      <c r="K26" s="155"/>
-      <c r="L26" s="155"/>
-      <c r="M26" s="155"/>
-      <c r="N26" s="155"/>
-      <c r="O26" s="155"/>
-      <c r="P26" s="155"/>
-      <c r="Q26" s="155"/>
-      <c r="R26" s="155"/>
+      <c r="B26" s="139"/>
+      <c r="C26" s="139"/>
+      <c r="D26" s="139"/>
+      <c r="E26" s="139"/>
+      <c r="F26" s="139"/>
+      <c r="G26" s="139"/>
+      <c r="H26" s="139"/>
+      <c r="I26" s="139"/>
+      <c r="J26" s="139"/>
+      <c r="K26" s="139"/>
+      <c r="L26" s="139"/>
+      <c r="M26" s="139"/>
+      <c r="N26" s="139"/>
+      <c r="O26" s="139"/>
+      <c r="P26" s="139"/>
+      <c r="Q26" s="139"/>
+      <c r="R26" s="139"/>
     </row>
     <row r="28" spans="1:195" ht="18">
-      <c r="B28" s="157"/>
-      <c r="C28" s="157"/>
-      <c r="D28" s="157"/>
-      <c r="E28" s="157"/>
-      <c r="F28" s="157"/>
-      <c r="G28" s="157"/>
-      <c r="H28" s="157"/>
-      <c r="I28" s="157"/>
-      <c r="J28" s="157"/>
-      <c r="K28" s="157"/>
-      <c r="L28" s="157"/>
-      <c r="M28" s="157"/>
-      <c r="N28" s="157"/>
-      <c r="O28" s="157"/>
-      <c r="P28" s="157"/>
-      <c r="Q28" s="157"/>
-      <c r="R28" s="157"/>
-      <c r="S28" s="156"/>
-      <c r="T28" s="156"/>
-      <c r="U28" s="156"/>
-      <c r="V28" s="156"/>
-      <c r="W28" s="156"/>
-      <c r="X28" s="156"/>
-      <c r="Y28" s="156"/>
-      <c r="Z28" s="156"/>
-      <c r="AA28" s="156"/>
-      <c r="AB28" s="156"/>
-      <c r="AC28" s="156"/>
-      <c r="AD28" s="156"/>
-      <c r="AE28" s="156"/>
-      <c r="AF28" s="156"/>
-      <c r="AG28" s="156"/>
-      <c r="AH28" s="156"/>
-      <c r="AI28" s="156"/>
-      <c r="AJ28" s="156"/>
-      <c r="AK28" s="156"/>
-      <c r="AL28" s="156"/>
-      <c r="AM28" s="156"/>
-      <c r="AN28" s="156"/>
-      <c r="AO28" s="156"/>
-      <c r="AP28" s="156"/>
-      <c r="AQ28" s="156"/>
-      <c r="AR28" s="156"/>
-      <c r="AS28" s="156"/>
-      <c r="AT28" s="156"/>
-      <c r="AU28" s="156"/>
-      <c r="AV28" s="156"/>
-      <c r="AW28" s="156"/>
-      <c r="AX28" s="156"/>
-      <c r="AY28" s="156"/>
-      <c r="AZ28" s="156"/>
-      <c r="BA28" s="156"/>
-      <c r="BB28" s="156"/>
-      <c r="BC28" s="156"/>
-      <c r="BD28" s="156"/>
-      <c r="BE28" s="156"/>
-      <c r="BF28" s="156"/>
-      <c r="BG28" s="156"/>
-      <c r="BH28" s="156"/>
-      <c r="BI28" s="156"/>
-      <c r="BJ28" s="156"/>
-      <c r="BK28" s="156"/>
-      <c r="BL28" s="156"/>
-      <c r="BM28" s="156"/>
-      <c r="BN28" s="156"/>
-      <c r="BO28" s="156"/>
-      <c r="BP28" s="156"/>
-      <c r="BQ28" s="156"/>
-      <c r="BR28" s="156"/>
-      <c r="BS28" s="156"/>
-      <c r="BT28" s="156"/>
-      <c r="BU28" s="156"/>
-      <c r="BV28" s="156"/>
-      <c r="BW28" s="156"/>
-      <c r="BX28" s="156"/>
-      <c r="BY28" s="156"/>
-      <c r="BZ28" s="156"/>
-      <c r="CA28" s="156"/>
-      <c r="CB28" s="156"/>
-      <c r="CC28" s="156"/>
-      <c r="CD28" s="156"/>
-      <c r="CE28" s="156"/>
-      <c r="CF28" s="156"/>
-      <c r="CG28" s="156"/>
-      <c r="CH28" s="156"/>
-      <c r="CI28" s="156"/>
-      <c r="CJ28" s="156"/>
-      <c r="CK28" s="156"/>
-      <c r="CL28" s="156"/>
-      <c r="CM28" s="156"/>
-      <c r="CN28" s="156"/>
-      <c r="CO28" s="156"/>
-      <c r="CP28" s="156"/>
-      <c r="CQ28" s="156"/>
-      <c r="CR28" s="156"/>
-      <c r="CS28" s="156"/>
-      <c r="CT28" s="156"/>
-      <c r="CU28" s="156"/>
-      <c r="CV28" s="156"/>
-      <c r="CW28" s="156"/>
-      <c r="CX28" s="156"/>
-      <c r="CY28" s="156"/>
-      <c r="CZ28" s="156"/>
-      <c r="DA28" s="156"/>
-      <c r="DB28" s="156"/>
-      <c r="DC28" s="156"/>
-      <c r="DD28" s="156"/>
-      <c r="DE28" s="156"/>
-      <c r="DF28" s="156"/>
-      <c r="DG28" s="156"/>
-      <c r="DH28" s="156"/>
-      <c r="DI28" s="156"/>
-      <c r="DJ28" s="156"/>
-      <c r="DK28" s="156"/>
-      <c r="DL28" s="156"/>
-      <c r="DM28" s="156"/>
-      <c r="DN28" s="156"/>
-      <c r="DO28" s="156"/>
-      <c r="DP28" s="156"/>
-      <c r="DQ28" s="156"/>
-      <c r="DR28" s="156"/>
-      <c r="DS28" s="156"/>
-      <c r="DT28" s="156"/>
-      <c r="DU28" s="156"/>
-      <c r="DV28" s="156"/>
-      <c r="DW28" s="156"/>
-      <c r="DX28" s="156"/>
-      <c r="DY28" s="156"/>
-      <c r="DZ28" s="156"/>
-      <c r="EA28" s="156"/>
-      <c r="EB28" s="156"/>
-      <c r="EC28" s="156"/>
-      <c r="ED28" s="156"/>
-      <c r="EE28" s="156"/>
-      <c r="EF28" s="156"/>
-      <c r="EG28" s="156"/>
-      <c r="EH28" s="156"/>
-      <c r="EI28" s="156"/>
-      <c r="EJ28" s="156"/>
-      <c r="EK28" s="156"/>
-      <c r="EL28" s="156"/>
-      <c r="EM28" s="156"/>
-      <c r="EN28" s="156"/>
-      <c r="EO28" s="156"/>
-      <c r="EP28" s="156"/>
-      <c r="EQ28" s="156"/>
-      <c r="ER28" s="156"/>
-      <c r="ES28" s="156"/>
-      <c r="ET28" s="156"/>
-      <c r="EU28" s="156"/>
-      <c r="EV28" s="156"/>
-      <c r="EW28" s="156"/>
-      <c r="EX28" s="156"/>
-      <c r="EY28" s="156"/>
-      <c r="EZ28" s="156"/>
-      <c r="FA28" s="156"/>
-      <c r="FB28" s="156"/>
-      <c r="FC28" s="156"/>
-      <c r="FD28" s="156"/>
-      <c r="FE28" s="156"/>
-      <c r="FF28" s="156"/>
-      <c r="FG28" s="156"/>
-      <c r="FH28" s="156"/>
-      <c r="FI28" s="156"/>
-      <c r="FJ28" s="156"/>
-      <c r="FK28" s="156"/>
-      <c r="FL28" s="156"/>
-      <c r="FM28" s="156"/>
-      <c r="FN28" s="156"/>
-      <c r="FO28" s="156"/>
-      <c r="FP28" s="156"/>
-      <c r="FQ28" s="156"/>
-      <c r="FR28" s="156"/>
-      <c r="FS28" s="156"/>
-      <c r="FT28" s="156"/>
-      <c r="FU28" s="156"/>
-      <c r="FV28" s="156"/>
-      <c r="FW28" s="156"/>
-      <c r="FX28" s="156"/>
-      <c r="FY28" s="156"/>
-      <c r="FZ28" s="156"/>
-      <c r="GA28" s="156"/>
-      <c r="GB28" s="156"/>
-      <c r="GC28" s="156"/>
-      <c r="GD28" s="156"/>
-      <c r="GE28" s="156"/>
-      <c r="GF28" s="156"/>
-      <c r="GG28" s="156"/>
-      <c r="GH28" s="156"/>
-      <c r="GI28" s="156"/>
-      <c r="GJ28" s="156"/>
-      <c r="GK28" s="156"/>
-      <c r="GL28" s="156"/>
+      <c r="B28" s="140"/>
+      <c r="C28" s="140"/>
+      <c r="D28" s="140"/>
+      <c r="E28" s="140"/>
+      <c r="F28" s="140"/>
+      <c r="G28" s="140"/>
+      <c r="H28" s="140"/>
+      <c r="I28" s="140"/>
+      <c r="J28" s="140"/>
+      <c r="K28" s="140"/>
+      <c r="L28" s="140"/>
+      <c r="M28" s="140"/>
+      <c r="N28" s="140"/>
+      <c r="O28" s="140"/>
+      <c r="P28" s="140"/>
+      <c r="Q28" s="140"/>
+      <c r="R28" s="140"/>
+      <c r="S28" s="138"/>
+      <c r="T28" s="138"/>
+      <c r="U28" s="138"/>
+      <c r="V28" s="138"/>
+      <c r="W28" s="138"/>
+      <c r="X28" s="138"/>
+      <c r="Y28" s="138"/>
+      <c r="Z28" s="138"/>
+      <c r="AA28" s="138"/>
+      <c r="AB28" s="138"/>
+      <c r="AC28" s="138"/>
+      <c r="AD28" s="138"/>
+      <c r="AE28" s="138"/>
+      <c r="AF28" s="138"/>
+      <c r="AG28" s="138"/>
+      <c r="AH28" s="138"/>
+      <c r="AI28" s="138"/>
+      <c r="AJ28" s="138"/>
+      <c r="AK28" s="138"/>
+      <c r="AL28" s="138"/>
+      <c r="AM28" s="138"/>
+      <c r="AN28" s="138"/>
+      <c r="AO28" s="138"/>
+      <c r="AP28" s="138"/>
+      <c r="AQ28" s="138"/>
+      <c r="AR28" s="138"/>
+      <c r="AS28" s="138"/>
+      <c r="AT28" s="138"/>
+      <c r="AU28" s="138"/>
+      <c r="AV28" s="138"/>
+      <c r="AW28" s="138"/>
+      <c r="AX28" s="138"/>
+      <c r="AY28" s="138"/>
+      <c r="AZ28" s="138"/>
+      <c r="BA28" s="138"/>
+      <c r="BB28" s="138"/>
+      <c r="BC28" s="138"/>
+      <c r="BD28" s="138"/>
+      <c r="BE28" s="138"/>
+      <c r="BF28" s="138"/>
+      <c r="BG28" s="138"/>
+      <c r="BH28" s="138"/>
+      <c r="BI28" s="138"/>
+      <c r="BJ28" s="138"/>
+      <c r="BK28" s="138"/>
+      <c r="BL28" s="138"/>
+      <c r="BM28" s="138"/>
+      <c r="BN28" s="138"/>
+      <c r="BO28" s="138"/>
+      <c r="BP28" s="138"/>
+      <c r="BQ28" s="138"/>
+      <c r="BR28" s="138"/>
+      <c r="BS28" s="138"/>
+      <c r="BT28" s="138"/>
+      <c r="BU28" s="138"/>
+      <c r="BV28" s="138"/>
+      <c r="BW28" s="138"/>
+      <c r="BX28" s="138"/>
+      <c r="BY28" s="138"/>
+      <c r="BZ28" s="138"/>
+      <c r="CA28" s="138"/>
+      <c r="CB28" s="138"/>
+      <c r="CC28" s="138"/>
+      <c r="CD28" s="138"/>
+      <c r="CE28" s="138"/>
+      <c r="CF28" s="138"/>
+      <c r="CG28" s="138"/>
+      <c r="CH28" s="138"/>
+      <c r="CI28" s="138"/>
+      <c r="CJ28" s="138"/>
+      <c r="CK28" s="138"/>
+      <c r="CL28" s="138"/>
+      <c r="CM28" s="138"/>
+      <c r="CN28" s="138"/>
+      <c r="CO28" s="138"/>
+      <c r="CP28" s="138"/>
+      <c r="CQ28" s="138"/>
+      <c r="CR28" s="138"/>
+      <c r="CS28" s="138"/>
+      <c r="CT28" s="138"/>
+      <c r="CU28" s="138"/>
+      <c r="CV28" s="138"/>
+      <c r="CW28" s="138"/>
+      <c r="CX28" s="138"/>
+      <c r="CY28" s="138"/>
+      <c r="CZ28" s="138"/>
+      <c r="DA28" s="138"/>
+      <c r="DB28" s="138"/>
+      <c r="DC28" s="138"/>
+      <c r="DD28" s="138"/>
+      <c r="DE28" s="138"/>
+      <c r="DF28" s="138"/>
+      <c r="DG28" s="138"/>
+      <c r="DH28" s="138"/>
+      <c r="DI28" s="138"/>
+      <c r="DJ28" s="138"/>
+      <c r="DK28" s="138"/>
+      <c r="DL28" s="138"/>
+      <c r="DM28" s="138"/>
+      <c r="DN28" s="138"/>
+      <c r="DO28" s="138"/>
+      <c r="DP28" s="138"/>
+      <c r="DQ28" s="138"/>
+      <c r="DR28" s="138"/>
+      <c r="DS28" s="138"/>
+      <c r="DT28" s="138"/>
+      <c r="DU28" s="138"/>
+      <c r="DV28" s="138"/>
+      <c r="DW28" s="138"/>
+      <c r="DX28" s="138"/>
+      <c r="DY28" s="138"/>
+      <c r="DZ28" s="138"/>
+      <c r="EA28" s="138"/>
+      <c r="EB28" s="138"/>
+      <c r="EC28" s="138"/>
+      <c r="ED28" s="138"/>
+      <c r="EE28" s="138"/>
+      <c r="EF28" s="138"/>
+      <c r="EG28" s="138"/>
+      <c r="EH28" s="138"/>
+      <c r="EI28" s="138"/>
+      <c r="EJ28" s="138"/>
+      <c r="EK28" s="138"/>
+      <c r="EL28" s="138"/>
+      <c r="EM28" s="138"/>
+      <c r="EN28" s="138"/>
+      <c r="EO28" s="138"/>
+      <c r="EP28" s="138"/>
+      <c r="EQ28" s="138"/>
+      <c r="ER28" s="138"/>
+      <c r="ES28" s="138"/>
+      <c r="ET28" s="138"/>
+      <c r="EU28" s="138"/>
+      <c r="EV28" s="138"/>
+      <c r="EW28" s="138"/>
+      <c r="EX28" s="138"/>
+      <c r="EY28" s="138"/>
+      <c r="EZ28" s="138"/>
+      <c r="FA28" s="138"/>
+      <c r="FB28" s="138"/>
+      <c r="FC28" s="138"/>
+      <c r="FD28" s="138"/>
+      <c r="FE28" s="138"/>
+      <c r="FF28" s="138"/>
+      <c r="FG28" s="138"/>
+      <c r="FH28" s="138"/>
+      <c r="FI28" s="138"/>
+      <c r="FJ28" s="138"/>
+      <c r="FK28" s="138"/>
+      <c r="FL28" s="138"/>
+      <c r="FM28" s="138"/>
+      <c r="FN28" s="138"/>
+      <c r="FO28" s="138"/>
+      <c r="FP28" s="138"/>
+      <c r="FQ28" s="138"/>
+      <c r="FR28" s="138"/>
+      <c r="FS28" s="138"/>
+      <c r="FT28" s="138"/>
+      <c r="FU28" s="138"/>
+      <c r="FV28" s="138"/>
+      <c r="FW28" s="138"/>
+      <c r="FX28" s="138"/>
+      <c r="FY28" s="138"/>
+      <c r="FZ28" s="138"/>
+      <c r="GA28" s="138"/>
+      <c r="GB28" s="138"/>
+      <c r="GC28" s="138"/>
+      <c r="GD28" s="138"/>
+      <c r="GE28" s="138"/>
+      <c r="GF28" s="138"/>
+      <c r="GG28" s="138"/>
+      <c r="GH28" s="138"/>
+      <c r="GI28" s="138"/>
+      <c r="GJ28" s="138"/>
+      <c r="GK28" s="138"/>
+      <c r="GL28" s="138"/>
       <c r="GM28" s="120"/>
     </row>
     <row r="29" spans="1:195" ht="18">
-      <c r="B29" s="155"/>
-      <c r="C29" s="155"/>
-      <c r="D29" s="155"/>
-      <c r="E29" s="155"/>
-      <c r="F29" s="155"/>
-      <c r="G29" s="155"/>
-      <c r="H29" s="155"/>
-      <c r="I29" s="155"/>
-      <c r="J29" s="155"/>
-      <c r="K29" s="155"/>
-      <c r="L29" s="155"/>
-      <c r="M29" s="155"/>
-      <c r="N29" s="155"/>
-      <c r="O29" s="155"/>
-      <c r="P29" s="155"/>
-      <c r="Q29" s="155"/>
-      <c r="R29" s="155"/>
+      <c r="B29" s="139"/>
+      <c r="C29" s="139"/>
+      <c r="D29" s="139"/>
+      <c r="E29" s="139"/>
+      <c r="F29" s="139"/>
+      <c r="G29" s="139"/>
+      <c r="H29" s="139"/>
+      <c r="I29" s="139"/>
+      <c r="J29" s="139"/>
+      <c r="K29" s="139"/>
+      <c r="L29" s="139"/>
+      <c r="M29" s="139"/>
+      <c r="N29" s="139"/>
+      <c r="O29" s="139"/>
+      <c r="P29" s="139"/>
+      <c r="Q29" s="139"/>
+      <c r="R29" s="139"/>
     </row>
     <row r="30" spans="1:195" ht="13.5" customHeight="1">
-      <c r="A30" s="158"/>
-      <c r="B30" s="158"/>
-      <c r="C30" s="158"/>
-      <c r="D30" s="158"/>
-      <c r="E30" s="158"/>
-      <c r="F30" s="158"/>
-      <c r="G30" s="158"/>
-      <c r="H30" s="158"/>
-      <c r="I30" s="158"/>
-      <c r="J30" s="158"/>
+      <c r="A30" s="137"/>
+      <c r="B30" s="137"/>
+      <c r="C30" s="137"/>
+      <c r="D30" s="137"/>
+      <c r="E30" s="137"/>
+      <c r="F30" s="137"/>
+      <c r="G30" s="137"/>
+      <c r="H30" s="137"/>
+      <c r="I30" s="137"/>
+      <c r="J30" s="137"/>
       <c r="K30" s="121"/>
       <c r="L30" s="121"/>
       <c r="M30" s="121"/>
@@ -4924,16 +4925,16 @@
       <c r="R30" s="121"/>
     </row>
     <row r="31" spans="1:195" ht="13.5" customHeight="1">
-      <c r="A31" s="158"/>
-      <c r="B31" s="158"/>
-      <c r="C31" s="158"/>
-      <c r="D31" s="158"/>
-      <c r="E31" s="158"/>
-      <c r="F31" s="158"/>
-      <c r="G31" s="158"/>
-      <c r="H31" s="158"/>
-      <c r="I31" s="158"/>
-      <c r="J31" s="158"/>
+      <c r="A31" s="137"/>
+      <c r="B31" s="137"/>
+      <c r="C31" s="137"/>
+      <c r="D31" s="137"/>
+      <c r="E31" s="137"/>
+      <c r="F31" s="137"/>
+      <c r="G31" s="137"/>
+      <c r="H31" s="137"/>
+      <c r="I31" s="137"/>
+      <c r="J31" s="137"/>
       <c r="K31" s="121"/>
       <c r="L31" s="121"/>
       <c r="M31" s="121"/>
@@ -4945,28 +4946,6 @@
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="A31:J31"/>
-    <mergeCell ref="DF28:DV28"/>
-    <mergeCell ref="DW28:EM28"/>
-    <mergeCell ref="EN28:FD28"/>
-    <mergeCell ref="B26:R26"/>
-    <mergeCell ref="FE28:FU28"/>
-    <mergeCell ref="FV28:GL28"/>
-    <mergeCell ref="B29:R29"/>
-    <mergeCell ref="S28:X28"/>
-    <mergeCell ref="Y28:AO28"/>
-    <mergeCell ref="AP28:BF28"/>
-    <mergeCell ref="BG28:BW28"/>
-    <mergeCell ref="BX28:CN28"/>
-    <mergeCell ref="CO28:DE28"/>
-    <mergeCell ref="B28:R28"/>
-    <mergeCell ref="B18:R18"/>
-    <mergeCell ref="B20:R20"/>
-    <mergeCell ref="B21:R21"/>
-    <mergeCell ref="B22:R22"/>
-    <mergeCell ref="B23:R23"/>
-    <mergeCell ref="B19:R19"/>
     <mergeCell ref="B14:R14"/>
     <mergeCell ref="B15:R15"/>
     <mergeCell ref="A16:J16"/>
@@ -4980,6 +4959,28 @@
     <mergeCell ref="C1:F3"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="I2:J2"/>
+    <mergeCell ref="B18:R18"/>
+    <mergeCell ref="B20:R20"/>
+    <mergeCell ref="B21:R21"/>
+    <mergeCell ref="B22:R22"/>
+    <mergeCell ref="B23:R23"/>
+    <mergeCell ref="B19:R19"/>
+    <mergeCell ref="B26:R26"/>
+    <mergeCell ref="FE28:FU28"/>
+    <mergeCell ref="FV28:GL28"/>
+    <mergeCell ref="B29:R29"/>
+    <mergeCell ref="S28:X28"/>
+    <mergeCell ref="Y28:AO28"/>
+    <mergeCell ref="AP28:BF28"/>
+    <mergeCell ref="BG28:BW28"/>
+    <mergeCell ref="BX28:CN28"/>
+    <mergeCell ref="CO28:DE28"/>
+    <mergeCell ref="B28:R28"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="A31:J31"/>
+    <mergeCell ref="DF28:DV28"/>
+    <mergeCell ref="DW28:EM28"/>
+    <mergeCell ref="EN28:FD28"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.196850393700787" right="0.196850393700787" top="0.39370078740157499" bottom="0" header="0" footer="0"/>
@@ -5534,10 +5535,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="12" customHeight="1">
-      <c r="A1" s="165" t="s">
+      <c r="A1" s="166" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="165"/>
+      <c r="B1" s="166"/>
       <c r="C1" s="31" t="s">
         <v>1</v>
       </c>
@@ -5564,8 +5565,8 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="12" customHeight="1">
-      <c r="A2" s="165"/>
-      <c r="B2" s="165"/>
+      <c r="A2" s="166"/>
+      <c r="B2" s="166"/>
       <c r="C2" s="31" t="s">
         <v>2</v>
       </c>
@@ -5604,14 +5605,14 @@
       <c r="D4" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="166" t="s">
+      <c r="E4" s="167" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="166"/>
-      <c r="G4" s="166"/>
-      <c r="H4" s="166"/>
-      <c r="I4" s="166"/>
-      <c r="J4" s="166"/>
+      <c r="F4" s="167"/>
+      <c r="G4" s="167"/>
+      <c r="H4" s="167"/>
+      <c r="I4" s="167"/>
+      <c r="J4" s="167"/>
     </row>
     <row r="5" spans="1:10" s="25" customFormat="1" ht="24" customHeight="1">
       <c r="A5" s="128">
@@ -5626,14 +5627,14 @@
       <c r="D5" s="130" t="s">
         <v>161</v>
       </c>
-      <c r="E5" s="167" t="s">
+      <c r="E5" s="168" t="s">
         <v>230</v>
       </c>
-      <c r="F5" s="168"/>
-      <c r="G5" s="168"/>
-      <c r="H5" s="168"/>
-      <c r="I5" s="168"/>
-      <c r="J5" s="168"/>
+      <c r="F5" s="169"/>
+      <c r="G5" s="169"/>
+      <c r="H5" s="169"/>
+      <c r="I5" s="169"/>
+      <c r="J5" s="169"/>
     </row>
     <row r="6" spans="1:10" ht="12.75">
       <c r="A6" s="91">
@@ -5644,12 +5645,12 @@
       </c>
       <c r="C6" s="78"/>
       <c r="D6" s="65"/>
-      <c r="E6" s="169"/>
-      <c r="F6" s="170"/>
-      <c r="G6" s="170"/>
-      <c r="H6" s="170"/>
-      <c r="I6" s="170"/>
-      <c r="J6" s="171"/>
+      <c r="E6" s="170"/>
+      <c r="F6" s="171"/>
+      <c r="G6" s="171"/>
+      <c r="H6" s="171"/>
+      <c r="I6" s="171"/>
+      <c r="J6" s="172"/>
     </row>
     <row r="7" spans="1:10" ht="12" customHeight="1">
       <c r="A7" s="92">
@@ -5660,12 +5661,12 @@
       </c>
       <c r="C7" s="79"/>
       <c r="D7" s="40"/>
-      <c r="E7" s="159"/>
-      <c r="F7" s="160"/>
-      <c r="G7" s="160"/>
-      <c r="H7" s="160"/>
-      <c r="I7" s="160"/>
-      <c r="J7" s="161"/>
+      <c r="E7" s="160"/>
+      <c r="F7" s="161"/>
+      <c r="G7" s="161"/>
+      <c r="H7" s="161"/>
+      <c r="I7" s="161"/>
+      <c r="J7" s="162"/>
     </row>
     <row r="8" spans="1:10" ht="12" customHeight="1">
       <c r="A8" s="93">
@@ -5676,12 +5677,12 @@
       </c>
       <c r="C8" s="79"/>
       <c r="D8" s="40"/>
-      <c r="E8" s="162"/>
-      <c r="F8" s="163"/>
-      <c r="G8" s="163"/>
-      <c r="H8" s="163"/>
-      <c r="I8" s="163"/>
-      <c r="J8" s="164"/>
+      <c r="E8" s="163"/>
+      <c r="F8" s="164"/>
+      <c r="G8" s="164"/>
+      <c r="H8" s="164"/>
+      <c r="I8" s="164"/>
+      <c r="J8" s="165"/>
     </row>
     <row r="9" spans="1:10" ht="12" customHeight="1">
       <c r="A9" s="94">
@@ -5692,12 +5693,12 @@
       </c>
       <c r="C9" s="79"/>
       <c r="D9" s="40"/>
-      <c r="E9" s="159"/>
-      <c r="F9" s="160"/>
-      <c r="G9" s="160"/>
-      <c r="H9" s="160"/>
-      <c r="I9" s="160"/>
-      <c r="J9" s="161"/>
+      <c r="E9" s="160"/>
+      <c r="F9" s="161"/>
+      <c r="G9" s="161"/>
+      <c r="H9" s="161"/>
+      <c r="I9" s="161"/>
+      <c r="J9" s="162"/>
     </row>
     <row r="10" spans="1:10" ht="12" customHeight="1">
       <c r="A10" s="95">
@@ -5708,12 +5709,12 @@
       </c>
       <c r="C10" s="79"/>
       <c r="D10" s="40"/>
-      <c r="E10" s="159"/>
-      <c r="F10" s="160"/>
-      <c r="G10" s="160"/>
-      <c r="H10" s="160"/>
-      <c r="I10" s="160"/>
-      <c r="J10" s="161"/>
+      <c r="E10" s="160"/>
+      <c r="F10" s="161"/>
+      <c r="G10" s="161"/>
+      <c r="H10" s="161"/>
+      <c r="I10" s="161"/>
+      <c r="J10" s="162"/>
     </row>
     <row r="11" spans="1:10" ht="12" customHeight="1">
       <c r="A11" s="96">
@@ -5724,12 +5725,12 @@
       </c>
       <c r="C11" s="79"/>
       <c r="D11" s="40"/>
-      <c r="E11" s="159"/>
-      <c r="F11" s="160"/>
-      <c r="G11" s="160"/>
-      <c r="H11" s="160"/>
-      <c r="I11" s="160"/>
-      <c r="J11" s="161"/>
+      <c r="E11" s="160"/>
+      <c r="F11" s="161"/>
+      <c r="G11" s="161"/>
+      <c r="H11" s="161"/>
+      <c r="I11" s="161"/>
+      <c r="J11" s="162"/>
     </row>
     <row r="12" spans="1:10" ht="12" customHeight="1">
       <c r="A12" s="97">
@@ -5740,12 +5741,12 @@
       </c>
       <c r="C12" s="79"/>
       <c r="D12" s="40"/>
-      <c r="E12" s="159"/>
-      <c r="F12" s="160"/>
-      <c r="G12" s="160"/>
-      <c r="H12" s="160"/>
-      <c r="I12" s="160"/>
-      <c r="J12" s="161"/>
+      <c r="E12" s="160"/>
+      <c r="F12" s="161"/>
+      <c r="G12" s="161"/>
+      <c r="H12" s="161"/>
+      <c r="I12" s="161"/>
+      <c r="J12" s="162"/>
     </row>
     <row r="13" spans="1:10" ht="12" customHeight="1">
       <c r="A13" s="98">
@@ -5756,12 +5757,12 @@
       </c>
       <c r="C13" s="79"/>
       <c r="D13" s="40"/>
-      <c r="E13" s="159"/>
-      <c r="F13" s="160"/>
-      <c r="G13" s="160"/>
-      <c r="H13" s="160"/>
-      <c r="I13" s="160"/>
-      <c r="J13" s="161"/>
+      <c r="E13" s="160"/>
+      <c r="F13" s="161"/>
+      <c r="G13" s="161"/>
+      <c r="H13" s="161"/>
+      <c r="I13" s="161"/>
+      <c r="J13" s="162"/>
     </row>
     <row r="14" spans="1:10" ht="12" customHeight="1">
       <c r="A14" s="99">
@@ -5772,12 +5773,12 @@
       </c>
       <c r="C14" s="79"/>
       <c r="D14" s="40"/>
-      <c r="E14" s="159"/>
-      <c r="F14" s="160"/>
-      <c r="G14" s="160"/>
-      <c r="H14" s="160"/>
-      <c r="I14" s="160"/>
-      <c r="J14" s="161"/>
+      <c r="E14" s="160"/>
+      <c r="F14" s="161"/>
+      <c r="G14" s="161"/>
+      <c r="H14" s="161"/>
+      <c r="I14" s="161"/>
+      <c r="J14" s="162"/>
     </row>
     <row r="15" spans="1:10" ht="12" customHeight="1">
       <c r="A15" s="40">
@@ -5788,12 +5789,12 @@
       </c>
       <c r="C15" s="79"/>
       <c r="D15" s="40"/>
-      <c r="E15" s="172"/>
-      <c r="F15" s="172"/>
-      <c r="G15" s="172"/>
-      <c r="H15" s="172"/>
-      <c r="I15" s="172"/>
-      <c r="J15" s="172"/>
+      <c r="E15" s="159"/>
+      <c r="F15" s="159"/>
+      <c r="G15" s="159"/>
+      <c r="H15" s="159"/>
+      <c r="I15" s="159"/>
+      <c r="J15" s="159"/>
     </row>
     <row r="16" spans="1:10" ht="12" customHeight="1">
       <c r="A16" s="91">
@@ -5804,12 +5805,12 @@
       </c>
       <c r="C16" s="79"/>
       <c r="D16" s="40"/>
-      <c r="E16" s="172"/>
-      <c r="F16" s="172"/>
-      <c r="G16" s="172"/>
-      <c r="H16" s="172"/>
-      <c r="I16" s="172"/>
-      <c r="J16" s="172"/>
+      <c r="E16" s="159"/>
+      <c r="F16" s="159"/>
+      <c r="G16" s="159"/>
+      <c r="H16" s="159"/>
+      <c r="I16" s="159"/>
+      <c r="J16" s="159"/>
     </row>
     <row r="17" spans="1:10" ht="12" customHeight="1">
       <c r="A17" s="92">
@@ -5820,12 +5821,12 @@
       </c>
       <c r="C17" s="79"/>
       <c r="D17" s="40"/>
-      <c r="E17" s="172"/>
-      <c r="F17" s="172"/>
-      <c r="G17" s="172"/>
-      <c r="H17" s="172"/>
-      <c r="I17" s="172"/>
-      <c r="J17" s="172"/>
+      <c r="E17" s="159"/>
+      <c r="F17" s="159"/>
+      <c r="G17" s="159"/>
+      <c r="H17" s="159"/>
+      <c r="I17" s="159"/>
+      <c r="J17" s="159"/>
     </row>
     <row r="18" spans="1:10" ht="12" customHeight="1">
       <c r="A18" s="93">
@@ -5836,12 +5837,12 @@
       </c>
       <c r="C18" s="79"/>
       <c r="D18" s="40"/>
-      <c r="E18" s="172"/>
-      <c r="F18" s="172"/>
-      <c r="G18" s="172"/>
-      <c r="H18" s="172"/>
-      <c r="I18" s="172"/>
-      <c r="J18" s="172"/>
+      <c r="E18" s="159"/>
+      <c r="F18" s="159"/>
+      <c r="G18" s="159"/>
+      <c r="H18" s="159"/>
+      <c r="I18" s="159"/>
+      <c r="J18" s="159"/>
     </row>
     <row r="19" spans="1:10" ht="12" customHeight="1">
       <c r="A19" s="94">
@@ -5852,12 +5853,12 @@
       </c>
       <c r="C19" s="79"/>
       <c r="D19" s="40"/>
-      <c r="E19" s="172"/>
-      <c r="F19" s="172"/>
-      <c r="G19" s="172"/>
-      <c r="H19" s="172"/>
-      <c r="I19" s="172"/>
-      <c r="J19" s="172"/>
+      <c r="E19" s="159"/>
+      <c r="F19" s="159"/>
+      <c r="G19" s="159"/>
+      <c r="H19" s="159"/>
+      <c r="I19" s="159"/>
+      <c r="J19" s="159"/>
     </row>
     <row r="20" spans="1:10" ht="12" customHeight="1">
       <c r="A20" s="95">
@@ -5868,12 +5869,12 @@
       </c>
       <c r="C20" s="79"/>
       <c r="D20" s="40"/>
-      <c r="E20" s="172"/>
-      <c r="F20" s="172"/>
-      <c r="G20" s="172"/>
-      <c r="H20" s="172"/>
-      <c r="I20" s="172"/>
-      <c r="J20" s="172"/>
+      <c r="E20" s="159"/>
+      <c r="F20" s="159"/>
+      <c r="G20" s="159"/>
+      <c r="H20" s="159"/>
+      <c r="I20" s="159"/>
+      <c r="J20" s="159"/>
     </row>
     <row r="21" spans="1:10" ht="12" customHeight="1">
       <c r="A21" s="96">
@@ -5884,12 +5885,12 @@
       </c>
       <c r="C21" s="79"/>
       <c r="D21" s="40"/>
-      <c r="E21" s="172"/>
-      <c r="F21" s="172"/>
-      <c r="G21" s="172"/>
-      <c r="H21" s="172"/>
-      <c r="I21" s="172"/>
-      <c r="J21" s="172"/>
+      <c r="E21" s="159"/>
+      <c r="F21" s="159"/>
+      <c r="G21" s="159"/>
+      <c r="H21" s="159"/>
+      <c r="I21" s="159"/>
+      <c r="J21" s="159"/>
     </row>
     <row r="22" spans="1:10" ht="12" customHeight="1">
       <c r="A22" s="97">
@@ -5900,12 +5901,12 @@
       </c>
       <c r="C22" s="79"/>
       <c r="D22" s="40"/>
-      <c r="E22" s="172"/>
-      <c r="F22" s="172"/>
-      <c r="G22" s="172"/>
-      <c r="H22" s="172"/>
-      <c r="I22" s="172"/>
-      <c r="J22" s="172"/>
+      <c r="E22" s="159"/>
+      <c r="F22" s="159"/>
+      <c r="G22" s="159"/>
+      <c r="H22" s="159"/>
+      <c r="I22" s="159"/>
+      <c r="J22" s="159"/>
     </row>
     <row r="23" spans="1:10" ht="12" customHeight="1">
       <c r="A23" s="98">
@@ -5916,12 +5917,12 @@
       </c>
       <c r="C23" s="79"/>
       <c r="D23" s="40"/>
-      <c r="E23" s="172"/>
-      <c r="F23" s="172"/>
-      <c r="G23" s="172"/>
-      <c r="H23" s="172"/>
-      <c r="I23" s="172"/>
-      <c r="J23" s="172"/>
+      <c r="E23" s="159"/>
+      <c r="F23" s="159"/>
+      <c r="G23" s="159"/>
+      <c r="H23" s="159"/>
+      <c r="I23" s="159"/>
+      <c r="J23" s="159"/>
     </row>
     <row r="24" spans="1:10" ht="12" customHeight="1">
       <c r="A24" s="99">
@@ -5932,12 +5933,12 @@
       </c>
       <c r="C24" s="79"/>
       <c r="D24" s="40"/>
-      <c r="E24" s="172"/>
-      <c r="F24" s="172"/>
-      <c r="G24" s="172"/>
-      <c r="H24" s="172"/>
-      <c r="I24" s="172"/>
-      <c r="J24" s="172"/>
+      <c r="E24" s="159"/>
+      <c r="F24" s="159"/>
+      <c r="G24" s="159"/>
+      <c r="H24" s="159"/>
+      <c r="I24" s="159"/>
+      <c r="J24" s="159"/>
     </row>
     <row r="25" spans="1:10" ht="12" customHeight="1">
       <c r="A25" s="40">
@@ -5948,12 +5949,12 @@
       </c>
       <c r="C25" s="79"/>
       <c r="D25" s="40"/>
-      <c r="E25" s="172"/>
-      <c r="F25" s="172"/>
-      <c r="G25" s="172"/>
-      <c r="H25" s="172"/>
-      <c r="I25" s="172"/>
-      <c r="J25" s="172"/>
+      <c r="E25" s="159"/>
+      <c r="F25" s="159"/>
+      <c r="G25" s="159"/>
+      <c r="H25" s="159"/>
+      <c r="I25" s="159"/>
+      <c r="J25" s="159"/>
     </row>
     <row r="26" spans="1:10" ht="12" customHeight="1">
       <c r="A26" s="40">
@@ -5964,12 +5965,12 @@
       </c>
       <c r="C26" s="79"/>
       <c r="D26" s="40"/>
-      <c r="E26" s="172"/>
-      <c r="F26" s="172"/>
-      <c r="G26" s="172"/>
-      <c r="H26" s="172"/>
-      <c r="I26" s="172"/>
-      <c r="J26" s="172"/>
+      <c r="E26" s="159"/>
+      <c r="F26" s="159"/>
+      <c r="G26" s="159"/>
+      <c r="H26" s="159"/>
+      <c r="I26" s="159"/>
+      <c r="J26" s="159"/>
     </row>
     <row r="27" spans="1:10" ht="12" customHeight="1">
       <c r="A27" s="91">
@@ -5980,12 +5981,12 @@
       </c>
       <c r="C27" s="79"/>
       <c r="D27" s="40"/>
-      <c r="E27" s="172"/>
-      <c r="F27" s="172"/>
-      <c r="G27" s="172"/>
-      <c r="H27" s="172"/>
-      <c r="I27" s="172"/>
-      <c r="J27" s="172"/>
+      <c r="E27" s="159"/>
+      <c r="F27" s="159"/>
+      <c r="G27" s="159"/>
+      <c r="H27" s="159"/>
+      <c r="I27" s="159"/>
+      <c r="J27" s="159"/>
     </row>
     <row r="28" spans="1:10" ht="12" customHeight="1">
       <c r="A28" s="92">
@@ -5996,12 +5997,12 @@
       </c>
       <c r="C28" s="79"/>
       <c r="D28" s="40"/>
-      <c r="E28" s="172"/>
-      <c r="F28" s="172"/>
-      <c r="G28" s="172"/>
-      <c r="H28" s="172"/>
-      <c r="I28" s="172"/>
-      <c r="J28" s="172"/>
+      <c r="E28" s="159"/>
+      <c r="F28" s="159"/>
+      <c r="G28" s="159"/>
+      <c r="H28" s="159"/>
+      <c r="I28" s="159"/>
+      <c r="J28" s="159"/>
     </row>
     <row r="29" spans="1:10" ht="12" customHeight="1">
       <c r="A29" s="93">
@@ -6012,12 +6013,12 @@
       </c>
       <c r="C29" s="79"/>
       <c r="D29" s="40"/>
-      <c r="E29" s="172"/>
-      <c r="F29" s="172"/>
-      <c r="G29" s="172"/>
-      <c r="H29" s="172"/>
-      <c r="I29" s="172"/>
-      <c r="J29" s="172"/>
+      <c r="E29" s="159"/>
+      <c r="F29" s="159"/>
+      <c r="G29" s="159"/>
+      <c r="H29" s="159"/>
+      <c r="I29" s="159"/>
+      <c r="J29" s="159"/>
     </row>
     <row r="30" spans="1:10" ht="12" customHeight="1">
       <c r="A30" s="94">
@@ -6028,12 +6029,12 @@
       </c>
       <c r="C30" s="79"/>
       <c r="D30" s="40"/>
-      <c r="E30" s="172"/>
-      <c r="F30" s="172"/>
-      <c r="G30" s="172"/>
-      <c r="H30" s="172"/>
-      <c r="I30" s="172"/>
-      <c r="J30" s="172"/>
+      <c r="E30" s="159"/>
+      <c r="F30" s="159"/>
+      <c r="G30" s="159"/>
+      <c r="H30" s="159"/>
+      <c r="I30" s="159"/>
+      <c r="J30" s="159"/>
     </row>
     <row r="31" spans="1:10" ht="12" customHeight="1">
       <c r="A31" s="95">
@@ -6044,12 +6045,12 @@
       </c>
       <c r="C31" s="79"/>
       <c r="D31" s="40"/>
-      <c r="E31" s="172"/>
-      <c r="F31" s="172"/>
-      <c r="G31" s="172"/>
-      <c r="H31" s="172"/>
-      <c r="I31" s="172"/>
-      <c r="J31" s="172"/>
+      <c r="E31" s="159"/>
+      <c r="F31" s="159"/>
+      <c r="G31" s="159"/>
+      <c r="H31" s="159"/>
+      <c r="I31" s="159"/>
+      <c r="J31" s="159"/>
     </row>
     <row r="32" spans="1:10" ht="12" customHeight="1">
       <c r="A32" s="96">
@@ -6060,12 +6061,12 @@
       </c>
       <c r="C32" s="79"/>
       <c r="D32" s="40"/>
-      <c r="E32" s="172"/>
-      <c r="F32" s="172"/>
-      <c r="G32" s="172"/>
-      <c r="H32" s="172"/>
-      <c r="I32" s="172"/>
-      <c r="J32" s="172"/>
+      <c r="E32" s="159"/>
+      <c r="F32" s="159"/>
+      <c r="G32" s="159"/>
+      <c r="H32" s="159"/>
+      <c r="I32" s="159"/>
+      <c r="J32" s="159"/>
     </row>
     <row r="33" spans="1:10" ht="12" customHeight="1">
       <c r="A33" s="97">
@@ -6076,12 +6077,12 @@
       </c>
       <c r="C33" s="79"/>
       <c r="D33" s="40"/>
-      <c r="E33" s="172"/>
-      <c r="F33" s="172"/>
-      <c r="G33" s="172"/>
-      <c r="H33" s="172"/>
-      <c r="I33" s="172"/>
-      <c r="J33" s="172"/>
+      <c r="E33" s="159"/>
+      <c r="F33" s="159"/>
+      <c r="G33" s="159"/>
+      <c r="H33" s="159"/>
+      <c r="I33" s="159"/>
+      <c r="J33" s="159"/>
     </row>
     <row r="34" spans="1:10" ht="12" customHeight="1">
       <c r="A34" s="98">
@@ -6092,12 +6093,12 @@
       </c>
       <c r="C34" s="79"/>
       <c r="D34" s="40"/>
-      <c r="E34" s="172"/>
-      <c r="F34" s="172"/>
-      <c r="G34" s="172"/>
-      <c r="H34" s="172"/>
-      <c r="I34" s="172"/>
-      <c r="J34" s="172"/>
+      <c r="E34" s="159"/>
+      <c r="F34" s="159"/>
+      <c r="G34" s="159"/>
+      <c r="H34" s="159"/>
+      <c r="I34" s="159"/>
+      <c r="J34" s="159"/>
     </row>
     <row r="35" spans="1:10" ht="12" customHeight="1">
       <c r="A35" s="99">
@@ -6108,12 +6109,12 @@
       </c>
       <c r="C35" s="79"/>
       <c r="D35" s="40"/>
-      <c r="E35" s="172"/>
-      <c r="F35" s="172"/>
-      <c r="G35" s="172"/>
-      <c r="H35" s="172"/>
-      <c r="I35" s="172"/>
-      <c r="J35" s="172"/>
+      <c r="E35" s="159"/>
+      <c r="F35" s="159"/>
+      <c r="G35" s="159"/>
+      <c r="H35" s="159"/>
+      <c r="I35" s="159"/>
+      <c r="J35" s="159"/>
     </row>
     <row r="36" spans="1:10" ht="12" customHeight="1">
       <c r="A36" s="40">
@@ -6124,12 +6125,12 @@
       </c>
       <c r="C36" s="79"/>
       <c r="D36" s="40"/>
-      <c r="E36" s="172"/>
-      <c r="F36" s="172"/>
-      <c r="G36" s="172"/>
-      <c r="H36" s="172"/>
-      <c r="I36" s="172"/>
-      <c r="J36" s="172"/>
+      <c r="E36" s="159"/>
+      <c r="F36" s="159"/>
+      <c r="G36" s="159"/>
+      <c r="H36" s="159"/>
+      <c r="I36" s="159"/>
+      <c r="J36" s="159"/>
     </row>
     <row r="37" spans="1:10" ht="12" customHeight="1">
       <c r="A37" s="91">
@@ -6140,12 +6141,12 @@
       </c>
       <c r="C37" s="79"/>
       <c r="D37" s="40"/>
-      <c r="E37" s="172"/>
-      <c r="F37" s="172"/>
-      <c r="G37" s="172"/>
-      <c r="H37" s="172"/>
-      <c r="I37" s="172"/>
-      <c r="J37" s="172"/>
+      <c r="E37" s="159"/>
+      <c r="F37" s="159"/>
+      <c r="G37" s="159"/>
+      <c r="H37" s="159"/>
+      <c r="I37" s="159"/>
+      <c r="J37" s="159"/>
     </row>
     <row r="38" spans="1:10" ht="12" customHeight="1">
       <c r="A38" s="92">
@@ -6156,12 +6157,12 @@
       </c>
       <c r="C38" s="79"/>
       <c r="D38" s="40"/>
-      <c r="E38" s="172"/>
-      <c r="F38" s="172"/>
-      <c r="G38" s="172"/>
-      <c r="H38" s="172"/>
-      <c r="I38" s="172"/>
-      <c r="J38" s="172"/>
+      <c r="E38" s="159"/>
+      <c r="F38" s="159"/>
+      <c r="G38" s="159"/>
+      <c r="H38" s="159"/>
+      <c r="I38" s="159"/>
+      <c r="J38" s="159"/>
     </row>
     <row r="39" spans="1:10" ht="12" customHeight="1">
       <c r="A39" s="93">
@@ -6172,12 +6173,12 @@
       </c>
       <c r="C39" s="79"/>
       <c r="D39" s="40"/>
-      <c r="E39" s="172"/>
-      <c r="F39" s="172"/>
-      <c r="G39" s="172"/>
-      <c r="H39" s="172"/>
-      <c r="I39" s="172"/>
-      <c r="J39" s="172"/>
+      <c r="E39" s="159"/>
+      <c r="F39" s="159"/>
+      <c r="G39" s="159"/>
+      <c r="H39" s="159"/>
+      <c r="I39" s="159"/>
+      <c r="J39" s="159"/>
     </row>
     <row r="40" spans="1:10" ht="12" customHeight="1">
       <c r="A40" s="94">
@@ -6188,12 +6189,12 @@
       </c>
       <c r="C40" s="79"/>
       <c r="D40" s="40"/>
-      <c r="E40" s="172"/>
-      <c r="F40" s="172"/>
-      <c r="G40" s="172"/>
-      <c r="H40" s="172"/>
-      <c r="I40" s="172"/>
-      <c r="J40" s="172"/>
+      <c r="E40" s="159"/>
+      <c r="F40" s="159"/>
+      <c r="G40" s="159"/>
+      <c r="H40" s="159"/>
+      <c r="I40" s="159"/>
+      <c r="J40" s="159"/>
     </row>
     <row r="41" spans="1:10" ht="12" customHeight="1">
       <c r="A41" s="95">
@@ -6204,12 +6205,12 @@
       </c>
       <c r="C41" s="79"/>
       <c r="D41" s="40"/>
-      <c r="E41" s="172"/>
-      <c r="F41" s="172"/>
-      <c r="G41" s="172"/>
-      <c r="H41" s="172"/>
-      <c r="I41" s="172"/>
-      <c r="J41" s="172"/>
+      <c r="E41" s="159"/>
+      <c r="F41" s="159"/>
+      <c r="G41" s="159"/>
+      <c r="H41" s="159"/>
+      <c r="I41" s="159"/>
+      <c r="J41" s="159"/>
     </row>
     <row r="42" spans="1:10" ht="12" customHeight="1">
       <c r="A42" s="96">
@@ -6220,32 +6221,23 @@
       </c>
       <c r="C42" s="79"/>
       <c r="D42" s="40"/>
-      <c r="E42" s="172"/>
-      <c r="F42" s="172"/>
-      <c r="G42" s="172"/>
-      <c r="H42" s="172"/>
-      <c r="I42" s="172"/>
-      <c r="J42" s="172"/>
+      <c r="E42" s="159"/>
+      <c r="F42" s="159"/>
+      <c r="G42" s="159"/>
+      <c r="H42" s="159"/>
+      <c r="I42" s="159"/>
+      <c r="J42" s="159"/>
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="E38:J38"/>
-    <mergeCell ref="E39:J39"/>
-    <mergeCell ref="E40:J40"/>
-    <mergeCell ref="E41:J41"/>
-    <mergeCell ref="E42:J42"/>
-    <mergeCell ref="E37:J37"/>
-    <mergeCell ref="E26:J26"/>
-    <mergeCell ref="E27:J27"/>
-    <mergeCell ref="E28:J28"/>
-    <mergeCell ref="E29:J29"/>
-    <mergeCell ref="E30:J30"/>
-    <mergeCell ref="E36:J36"/>
-    <mergeCell ref="E31:J31"/>
-    <mergeCell ref="E32:J32"/>
-    <mergeCell ref="E33:J33"/>
-    <mergeCell ref="E34:J34"/>
-    <mergeCell ref="E35:J35"/>
+    <mergeCell ref="E7:J7"/>
+    <mergeCell ref="E8:J8"/>
+    <mergeCell ref="E9:J9"/>
+    <mergeCell ref="E10:J10"/>
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="E4:J4"/>
+    <mergeCell ref="E5:J5"/>
+    <mergeCell ref="E6:J6"/>
     <mergeCell ref="E11:J11"/>
     <mergeCell ref="E12:J12"/>
     <mergeCell ref="E25:J25"/>
@@ -6261,14 +6253,23 @@
     <mergeCell ref="E22:J22"/>
     <mergeCell ref="E23:J23"/>
     <mergeCell ref="E24:J24"/>
-    <mergeCell ref="E7:J7"/>
-    <mergeCell ref="E8:J8"/>
-    <mergeCell ref="E9:J9"/>
-    <mergeCell ref="E10:J10"/>
-    <mergeCell ref="A1:B2"/>
-    <mergeCell ref="E4:J4"/>
-    <mergeCell ref="E5:J5"/>
-    <mergeCell ref="E6:J6"/>
+    <mergeCell ref="E37:J37"/>
+    <mergeCell ref="E26:J26"/>
+    <mergeCell ref="E27:J27"/>
+    <mergeCell ref="E28:J28"/>
+    <mergeCell ref="E29:J29"/>
+    <mergeCell ref="E30:J30"/>
+    <mergeCell ref="E36:J36"/>
+    <mergeCell ref="E31:J31"/>
+    <mergeCell ref="E32:J32"/>
+    <mergeCell ref="E33:J33"/>
+    <mergeCell ref="E34:J34"/>
+    <mergeCell ref="E35:J35"/>
+    <mergeCell ref="E38:J38"/>
+    <mergeCell ref="E39:J39"/>
+    <mergeCell ref="E40:J40"/>
+    <mergeCell ref="E41:J41"/>
+    <mergeCell ref="E42:J42"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1">
@@ -6293,8 +6294,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12:J43"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A16" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" customHeight="1"/>
@@ -6313,10 +6314,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="12" customHeight="1">
-      <c r="A1" s="165" t="s">
+      <c r="A1" s="166" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="165"/>
+      <c r="B1" s="166"/>
       <c r="C1" s="31" t="s">
         <v>1</v>
       </c>
@@ -6346,8 +6347,8 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="12" customHeight="1">
-      <c r="A2" s="165"/>
-      <c r="B2" s="165"/>
+      <c r="A2" s="166"/>
+      <c r="B2" s="166"/>
       <c r="C2" s="31" t="s">
         <v>2</v>
       </c>
@@ -6490,7 +6491,7 @@
       <c r="G12" s="43"/>
       <c r="H12" s="45"/>
       <c r="I12" s="176" t="s">
-        <v>237</v>
+        <v>242</v>
       </c>
       <c r="J12" s="177"/>
     </row>
@@ -6923,13 +6924,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="25" customFormat="1" ht="12" customHeight="1">
-      <c r="A1" s="165" t="s">
+      <c r="A1" s="166" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="165"/>
-      <c r="C1" s="165"/>
-      <c r="D1" s="165"/>
-      <c r="E1" s="165"/>
+      <c r="B1" s="166"/>
+      <c r="C1" s="166"/>
+      <c r="D1" s="166"/>
+      <c r="E1" s="166"/>
       <c r="F1" s="30" t="s">
         <v>1</v>
       </c>
@@ -6961,11 +6962,11 @@
       </c>
     </row>
     <row r="2" spans="1:16" s="25" customFormat="1" ht="12" customHeight="1">
-      <c r="A2" s="165"/>
-      <c r="B2" s="165"/>
-      <c r="C2" s="165"/>
-      <c r="D2" s="165"/>
-      <c r="E2" s="165"/>
+      <c r="A2" s="166"/>
+      <c r="B2" s="166"/>
+      <c r="C2" s="166"/>
+      <c r="D2" s="166"/>
+      <c r="E2" s="166"/>
       <c r="F2" s="30" t="s">
         <v>2</v>
       </c>
@@ -9439,7 +9440,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="25" customFormat="1" ht="12" customHeight="1">
-      <c r="A1" s="198" t="s">
+      <c r="A1" s="195" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="135"/>
@@ -9473,7 +9474,7 @@
       <c r="M1" s="52"/>
     </row>
     <row r="2" spans="1:13" s="25" customFormat="1" ht="12" customHeight="1">
-      <c r="A2" s="199"/>
+      <c r="A2" s="196"/>
       <c r="B2" s="136"/>
       <c r="C2" s="125"/>
       <c r="D2" s="31" t="s">
@@ -9523,15 +9524,15 @@
       <c r="F4" s="101" t="s">
         <v>46</v>
       </c>
-      <c r="G4" s="165" t="s">
+      <c r="G4" s="166" t="s">
         <v>131</v>
       </c>
-      <c r="H4" s="165"/>
-      <c r="I4" s="165" t="s">
+      <c r="H4" s="166"/>
+      <c r="I4" s="166" t="s">
         <v>48</v>
       </c>
-      <c r="J4" s="165"/>
-      <c r="K4" s="165"/>
+      <c r="J4" s="166"/>
+      <c r="K4" s="166"/>
     </row>
     <row r="5" spans="1:13" s="34" customFormat="1" ht="27" customHeight="1">
       <c r="A5" s="33">
@@ -9545,18 +9546,18 @@
       </c>
       <c r="D5" s="33"/>
       <c r="E5" s="131" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F5" s="32"/>
-      <c r="G5" s="196" t="s">
-        <v>238</v>
-      </c>
-      <c r="H5" s="197"/>
-      <c r="I5" s="193" t="s">
+      <c r="G5" s="193" t="s">
+        <v>237</v>
+      </c>
+      <c r="H5" s="194"/>
+      <c r="I5" s="197" t="s">
         <v>219</v>
       </c>
-      <c r="J5" s="194"/>
-      <c r="K5" s="195"/>
+      <c r="J5" s="198"/>
+      <c r="K5" s="199"/>
     </row>
     <row r="6" spans="1:13" s="34" customFormat="1" ht="24" customHeight="1">
       <c r="A6" s="33">
@@ -9573,15 +9574,15 @@
         <v>134</v>
       </c>
       <c r="F6" s="32"/>
-      <c r="G6" s="196" t="s">
+      <c r="G6" s="193" t="s">
         <v>216</v>
       </c>
-      <c r="H6" s="197"/>
-      <c r="I6" s="193" t="s">
+      <c r="H6" s="194"/>
+      <c r="I6" s="197" t="s">
         <v>181</v>
       </c>
-      <c r="J6" s="194"/>
-      <c r="K6" s="195"/>
+      <c r="J6" s="198"/>
+      <c r="K6" s="199"/>
     </row>
     <row r="7" spans="1:13" s="34" customFormat="1" ht="11.25" customHeight="1">
       <c r="A7" s="33">
@@ -9592,11 +9593,11 @@
       <c r="D7" s="33"/>
       <c r="E7" s="33"/>
       <c r="F7" s="32"/>
-      <c r="G7" s="196"/>
-      <c r="H7" s="197"/>
-      <c r="I7" s="193"/>
-      <c r="J7" s="194"/>
-      <c r="K7" s="195"/>
+      <c r="G7" s="193"/>
+      <c r="H7" s="194"/>
+      <c r="I7" s="197"/>
+      <c r="J7" s="198"/>
+      <c r="K7" s="199"/>
     </row>
     <row r="8" spans="1:13" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A8" s="33">
@@ -9607,11 +9608,11 @@
       <c r="D8" s="33"/>
       <c r="E8" s="33"/>
       <c r="F8" s="32"/>
-      <c r="G8" s="196"/>
-      <c r="H8" s="197"/>
-      <c r="I8" s="193"/>
-      <c r="J8" s="194"/>
-      <c r="K8" s="195"/>
+      <c r="G8" s="193"/>
+      <c r="H8" s="194"/>
+      <c r="I8" s="197"/>
+      <c r="J8" s="198"/>
+      <c r="K8" s="199"/>
     </row>
     <row r="9" spans="1:13" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A9" s="33">
@@ -9622,11 +9623,11 @@
       <c r="D9" s="33"/>
       <c r="E9" s="33"/>
       <c r="F9" s="32"/>
-      <c r="G9" s="196"/>
-      <c r="H9" s="197"/>
-      <c r="I9" s="193"/>
-      <c r="J9" s="194"/>
-      <c r="K9" s="195"/>
+      <c r="G9" s="193"/>
+      <c r="H9" s="194"/>
+      <c r="I9" s="197"/>
+      <c r="J9" s="198"/>
+      <c r="K9" s="199"/>
     </row>
     <row r="10" spans="1:13" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A10" s="33">
@@ -9637,11 +9638,11 @@
       <c r="D10" s="33"/>
       <c r="E10" s="33"/>
       <c r="F10" s="32"/>
-      <c r="G10" s="196"/>
-      <c r="H10" s="197"/>
-      <c r="I10" s="193"/>
-      <c r="J10" s="194"/>
-      <c r="K10" s="195"/>
+      <c r="G10" s="193"/>
+      <c r="H10" s="194"/>
+      <c r="I10" s="197"/>
+      <c r="J10" s="198"/>
+      <c r="K10" s="199"/>
     </row>
     <row r="11" spans="1:13" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A11" s="33">
@@ -9652,11 +9653,11 @@
       <c r="D11" s="33"/>
       <c r="E11" s="33"/>
       <c r="F11" s="32"/>
-      <c r="G11" s="196"/>
-      <c r="H11" s="197"/>
-      <c r="I11" s="193"/>
-      <c r="J11" s="194"/>
-      <c r="K11" s="195"/>
+      <c r="G11" s="193"/>
+      <c r="H11" s="194"/>
+      <c r="I11" s="197"/>
+      <c r="J11" s="198"/>
+      <c r="K11" s="199"/>
     </row>
     <row r="12" spans="1:13" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A12" s="33">
@@ -9667,11 +9668,11 @@
       <c r="D12" s="33"/>
       <c r="E12" s="33"/>
       <c r="F12" s="32"/>
-      <c r="G12" s="196"/>
-      <c r="H12" s="197"/>
-      <c r="I12" s="193"/>
-      <c r="J12" s="194"/>
-      <c r="K12" s="195"/>
+      <c r="G12" s="193"/>
+      <c r="H12" s="194"/>
+      <c r="I12" s="197"/>
+      <c r="J12" s="198"/>
+      <c r="K12" s="199"/>
     </row>
     <row r="13" spans="1:13" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A13" s="33">
@@ -9682,11 +9683,11 @@
       <c r="D13" s="33"/>
       <c r="E13" s="33"/>
       <c r="F13" s="32"/>
-      <c r="G13" s="196"/>
-      <c r="H13" s="197"/>
-      <c r="I13" s="193"/>
-      <c r="J13" s="194"/>
-      <c r="K13" s="195"/>
+      <c r="G13" s="193"/>
+      <c r="H13" s="194"/>
+      <c r="I13" s="197"/>
+      <c r="J13" s="198"/>
+      <c r="K13" s="199"/>
     </row>
     <row r="14" spans="1:13" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A14" s="33">
@@ -9697,11 +9698,11 @@
       <c r="D14" s="33"/>
       <c r="E14" s="33"/>
       <c r="F14" s="32"/>
-      <c r="G14" s="196"/>
-      <c r="H14" s="197"/>
-      <c r="I14" s="193"/>
-      <c r="J14" s="194"/>
-      <c r="K14" s="195"/>
+      <c r="G14" s="193"/>
+      <c r="H14" s="194"/>
+      <c r="I14" s="197"/>
+      <c r="J14" s="198"/>
+      <c r="K14" s="199"/>
     </row>
     <row r="15" spans="1:13" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A15" s="33">
@@ -9712,11 +9713,11 @@
       <c r="D15" s="33"/>
       <c r="E15" s="33"/>
       <c r="F15" s="32"/>
-      <c r="G15" s="196"/>
-      <c r="H15" s="197"/>
-      <c r="I15" s="193"/>
-      <c r="J15" s="194"/>
-      <c r="K15" s="195"/>
+      <c r="G15" s="193"/>
+      <c r="H15" s="194"/>
+      <c r="I15" s="197"/>
+      <c r="J15" s="198"/>
+      <c r="K15" s="199"/>
     </row>
     <row r="16" spans="1:13" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A16" s="33">
@@ -9727,11 +9728,11 @@
       <c r="D16" s="33"/>
       <c r="E16" s="33"/>
       <c r="F16" s="32"/>
-      <c r="G16" s="196"/>
-      <c r="H16" s="197"/>
-      <c r="I16" s="193"/>
-      <c r="J16" s="194"/>
-      <c r="K16" s="195"/>
+      <c r="G16" s="193"/>
+      <c r="H16" s="194"/>
+      <c r="I16" s="197"/>
+      <c r="J16" s="198"/>
+      <c r="K16" s="199"/>
     </row>
     <row r="17" spans="1:19" s="34" customFormat="1" ht="11.25">
       <c r="A17" s="33">
@@ -9742,11 +9743,11 @@
       <c r="D17" s="33"/>
       <c r="E17" s="33"/>
       <c r="F17" s="32"/>
-      <c r="G17" s="196"/>
-      <c r="H17" s="197"/>
-      <c r="I17" s="193"/>
-      <c r="J17" s="194"/>
-      <c r="K17" s="195"/>
+      <c r="G17" s="193"/>
+      <c r="H17" s="194"/>
+      <c r="I17" s="197"/>
+      <c r="J17" s="198"/>
+      <c r="K17" s="199"/>
     </row>
     <row r="18" spans="1:19" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A18" s="33">
@@ -9757,11 +9758,11 @@
       <c r="D18" s="33"/>
       <c r="E18" s="33"/>
       <c r="F18" s="32"/>
-      <c r="G18" s="196"/>
-      <c r="H18" s="197"/>
-      <c r="I18" s="193"/>
-      <c r="J18" s="194"/>
-      <c r="K18" s="195"/>
+      <c r="G18" s="193"/>
+      <c r="H18" s="194"/>
+      <c r="I18" s="197"/>
+      <c r="J18" s="198"/>
+      <c r="K18" s="199"/>
     </row>
     <row r="19" spans="1:19" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A19" s="33">
@@ -9772,11 +9773,11 @@
       <c r="D19" s="33"/>
       <c r="E19" s="33"/>
       <c r="F19" s="32"/>
-      <c r="G19" s="196"/>
-      <c r="H19" s="197"/>
-      <c r="I19" s="193"/>
-      <c r="J19" s="194"/>
-      <c r="K19" s="195"/>
+      <c r="G19" s="193"/>
+      <c r="H19" s="194"/>
+      <c r="I19" s="197"/>
+      <c r="J19" s="198"/>
+      <c r="K19" s="199"/>
     </row>
     <row r="20" spans="1:19" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A20" s="33">
@@ -9787,11 +9788,11 @@
       <c r="D20" s="33"/>
       <c r="E20" s="33"/>
       <c r="F20" s="32"/>
-      <c r="G20" s="196"/>
-      <c r="H20" s="197"/>
-      <c r="I20" s="193"/>
-      <c r="J20" s="194"/>
-      <c r="K20" s="195"/>
+      <c r="G20" s="193"/>
+      <c r="H20" s="194"/>
+      <c r="I20" s="197"/>
+      <c r="J20" s="198"/>
+      <c r="K20" s="199"/>
     </row>
     <row r="21" spans="1:19" s="34" customFormat="1" ht="11.25">
       <c r="A21" s="33">
@@ -9802,11 +9803,11 @@
       <c r="D21" s="33"/>
       <c r="E21" s="33"/>
       <c r="F21" s="32"/>
-      <c r="G21" s="196"/>
-      <c r="H21" s="197"/>
-      <c r="I21" s="193"/>
-      <c r="J21" s="194"/>
-      <c r="K21" s="195"/>
+      <c r="G21" s="193"/>
+      <c r="H21" s="194"/>
+      <c r="I21" s="197"/>
+      <c r="J21" s="198"/>
+      <c r="K21" s="199"/>
     </row>
     <row r="22" spans="1:19" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A22" s="33">
@@ -9817,11 +9818,11 @@
       <c r="D22" s="33"/>
       <c r="E22" s="33"/>
       <c r="F22" s="32"/>
-      <c r="G22" s="159"/>
-      <c r="H22" s="161"/>
-      <c r="I22" s="193"/>
-      <c r="J22" s="194"/>
-      <c r="K22" s="195"/>
+      <c r="G22" s="160"/>
+      <c r="H22" s="162"/>
+      <c r="I22" s="197"/>
+      <c r="J22" s="198"/>
+      <c r="K22" s="199"/>
     </row>
     <row r="23" spans="1:19" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A23" s="33">
@@ -9832,11 +9833,11 @@
       <c r="D23" s="33"/>
       <c r="E23" s="33"/>
       <c r="F23" s="32"/>
-      <c r="G23" s="159"/>
-      <c r="H23" s="161"/>
-      <c r="I23" s="193"/>
-      <c r="J23" s="194"/>
-      <c r="K23" s="195"/>
+      <c r="G23" s="160"/>
+      <c r="H23" s="162"/>
+      <c r="I23" s="197"/>
+      <c r="J23" s="198"/>
+      <c r="K23" s="199"/>
     </row>
     <row r="24" spans="1:19" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A24" s="33">
@@ -9847,11 +9848,11 @@
       <c r="D24" s="33"/>
       <c r="E24" s="33"/>
       <c r="F24" s="32"/>
-      <c r="G24" s="159"/>
-      <c r="H24" s="161"/>
-      <c r="I24" s="193"/>
-      <c r="J24" s="194"/>
-      <c r="K24" s="195"/>
+      <c r="G24" s="160"/>
+      <c r="H24" s="162"/>
+      <c r="I24" s="197"/>
+      <c r="J24" s="198"/>
+      <c r="K24" s="199"/>
     </row>
     <row r="25" spans="1:19" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A25" s="33">
@@ -9862,11 +9863,11 @@
       <c r="D25" s="33"/>
       <c r="E25" s="33"/>
       <c r="F25" s="32"/>
-      <c r="G25" s="159"/>
-      <c r="H25" s="161"/>
-      <c r="I25" s="193"/>
-      <c r="J25" s="194"/>
-      <c r="K25" s="195"/>
+      <c r="G25" s="160"/>
+      <c r="H25" s="162"/>
+      <c r="I25" s="197"/>
+      <c r="J25" s="198"/>
+      <c r="K25" s="199"/>
     </row>
     <row r="26" spans="1:19" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A26" s="33">
@@ -9877,11 +9878,11 @@
       <c r="D26" s="33"/>
       <c r="E26" s="33"/>
       <c r="F26" s="32"/>
-      <c r="G26" s="159"/>
-      <c r="H26" s="161"/>
-      <c r="I26" s="193"/>
-      <c r="J26" s="194"/>
-      <c r="K26" s="195"/>
+      <c r="G26" s="160"/>
+      <c r="H26" s="162"/>
+      <c r="I26" s="197"/>
+      <c r="J26" s="198"/>
+      <c r="K26" s="199"/>
     </row>
     <row r="27" spans="1:19" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A27" s="33">
@@ -9892,11 +9893,11 @@
       <c r="D27" s="33"/>
       <c r="E27" s="33"/>
       <c r="F27" s="32"/>
-      <c r="G27" s="159"/>
-      <c r="H27" s="161"/>
-      <c r="I27" s="193"/>
-      <c r="J27" s="194"/>
-      <c r="K27" s="195"/>
+      <c r="G27" s="160"/>
+      <c r="H27" s="162"/>
+      <c r="I27" s="197"/>
+      <c r="J27" s="198"/>
+      <c r="K27" s="199"/>
     </row>
     <row r="28" spans="1:19" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A28" s="33">
@@ -9907,11 +9908,11 @@
       <c r="D28" s="33"/>
       <c r="E28" s="33"/>
       <c r="F28" s="32"/>
-      <c r="G28" s="159"/>
-      <c r="H28" s="161"/>
-      <c r="I28" s="193"/>
-      <c r="J28" s="194"/>
-      <c r="K28" s="195"/>
+      <c r="G28" s="160"/>
+      <c r="H28" s="162"/>
+      <c r="I28" s="197"/>
+      <c r="J28" s="198"/>
+      <c r="K28" s="199"/>
     </row>
     <row r="29" spans="1:19" s="34" customFormat="1" ht="12" customHeight="1">
       <c r="A29" s="33">
@@ -9922,11 +9923,11 @@
       <c r="D29" s="33"/>
       <c r="E29" s="33"/>
       <c r="F29" s="32"/>
-      <c r="G29" s="159"/>
-      <c r="H29" s="161"/>
-      <c r="I29" s="193"/>
-      <c r="J29" s="194"/>
-      <c r="K29" s="195"/>
+      <c r="G29" s="160"/>
+      <c r="H29" s="162"/>
+      <c r="I29" s="197"/>
+      <c r="J29" s="198"/>
+      <c r="K29" s="199"/>
     </row>
     <row r="30" spans="1:19" s="34" customFormat="1" ht="11.25" customHeight="1">
       <c r="A30" s="33">
@@ -9937,11 +9938,11 @@
       <c r="D30" s="33"/>
       <c r="E30" s="33"/>
       <c r="F30" s="32"/>
-      <c r="G30" s="159"/>
-      <c r="H30" s="161"/>
-      <c r="I30" s="193"/>
-      <c r="J30" s="194"/>
-      <c r="K30" s="195"/>
+      <c r="G30" s="160"/>
+      <c r="H30" s="162"/>
+      <c r="I30" s="197"/>
+      <c r="J30" s="198"/>
+      <c r="K30" s="199"/>
     </row>
     <row r="31" spans="1:19" s="34" customFormat="1" ht="11.25" customHeight="1">
       <c r="A31" s="33">
@@ -9952,11 +9953,11 @@
       <c r="D31" s="33"/>
       <c r="E31" s="33"/>
       <c r="F31" s="32"/>
-      <c r="G31" s="159"/>
-      <c r="H31" s="161"/>
-      <c r="I31" s="193"/>
-      <c r="J31" s="194"/>
-      <c r="K31" s="195"/>
+      <c r="G31" s="160"/>
+      <c r="H31" s="162"/>
+      <c r="I31" s="197"/>
+      <c r="J31" s="198"/>
+      <c r="K31" s="199"/>
     </row>
     <row r="32" spans="1:19" ht="11.25">
       <c r="A32" s="33">
@@ -9967,11 +9968,11 @@
       <c r="D32" s="33"/>
       <c r="E32" s="33"/>
       <c r="F32" s="32"/>
-      <c r="G32" s="159"/>
-      <c r="H32" s="161"/>
-      <c r="I32" s="193"/>
-      <c r="J32" s="194"/>
-      <c r="K32" s="195"/>
+      <c r="G32" s="160"/>
+      <c r="H32" s="162"/>
+      <c r="I32" s="197"/>
+      <c r="J32" s="198"/>
+      <c r="K32" s="199"/>
       <c r="M32" s="22"/>
       <c r="N32" s="22"/>
       <c r="O32" s="22"/>
@@ -9989,11 +9990,11 @@
       <c r="D33" s="33"/>
       <c r="E33" s="33"/>
       <c r="F33" s="32"/>
-      <c r="G33" s="159"/>
-      <c r="H33" s="161"/>
-      <c r="I33" s="193"/>
-      <c r="J33" s="194"/>
-      <c r="K33" s="195"/>
+      <c r="G33" s="160"/>
+      <c r="H33" s="162"/>
+      <c r="I33" s="197"/>
+      <c r="J33" s="198"/>
+      <c r="K33" s="199"/>
       <c r="M33" s="22"/>
       <c r="N33" s="22"/>
       <c r="O33" s="22"/>
@@ -10011,11 +10012,11 @@
       <c r="D34" s="33"/>
       <c r="E34" s="33"/>
       <c r="F34" s="32"/>
-      <c r="G34" s="159"/>
-      <c r="H34" s="161"/>
-      <c r="I34" s="193"/>
-      <c r="J34" s="194"/>
-      <c r="K34" s="195"/>
+      <c r="G34" s="160"/>
+      <c r="H34" s="162"/>
+      <c r="I34" s="197"/>
+      <c r="J34" s="198"/>
+      <c r="K34" s="199"/>
       <c r="M34" s="22"/>
       <c r="N34" s="22"/>
       <c r="O34" s="22"/>
@@ -10033,11 +10034,11 @@
       <c r="D35" s="33"/>
       <c r="E35" s="33"/>
       <c r="F35" s="32"/>
-      <c r="G35" s="159"/>
-      <c r="H35" s="161"/>
-      <c r="I35" s="193"/>
-      <c r="J35" s="194"/>
-      <c r="K35" s="195"/>
+      <c r="G35" s="160"/>
+      <c r="H35" s="162"/>
+      <c r="I35" s="197"/>
+      <c r="J35" s="198"/>
+      <c r="K35" s="199"/>
       <c r="M35" s="22"/>
       <c r="N35" s="22"/>
       <c r="O35" s="22"/>
@@ -10055,11 +10056,11 @@
       <c r="D36" s="33"/>
       <c r="E36" s="33"/>
       <c r="F36" s="32"/>
-      <c r="G36" s="159"/>
-      <c r="H36" s="161"/>
-      <c r="I36" s="193"/>
-      <c r="J36" s="194"/>
-      <c r="K36" s="195"/>
+      <c r="G36" s="160"/>
+      <c r="H36" s="162"/>
+      <c r="I36" s="197"/>
+      <c r="J36" s="198"/>
+      <c r="K36" s="199"/>
       <c r="M36" s="22"/>
       <c r="N36" s="22"/>
       <c r="O36" s="22"/>
@@ -10077,11 +10078,11 @@
       <c r="D37" s="33"/>
       <c r="E37" s="33"/>
       <c r="F37" s="32"/>
-      <c r="G37" s="159"/>
-      <c r="H37" s="161"/>
-      <c r="I37" s="193"/>
-      <c r="J37" s="194"/>
-      <c r="K37" s="195"/>
+      <c r="G37" s="160"/>
+      <c r="H37" s="162"/>
+      <c r="I37" s="197"/>
+      <c r="J37" s="198"/>
+      <c r="K37" s="199"/>
       <c r="M37" s="22"/>
       <c r="N37" s="22"/>
       <c r="O37" s="22"/>
@@ -10099,11 +10100,11 @@
       <c r="D38" s="33"/>
       <c r="E38" s="33"/>
       <c r="F38" s="32"/>
-      <c r="G38" s="159"/>
-      <c r="H38" s="161"/>
-      <c r="I38" s="193"/>
-      <c r="J38" s="194"/>
-      <c r="K38" s="195"/>
+      <c r="G38" s="160"/>
+      <c r="H38" s="162"/>
+      <c r="I38" s="197"/>
+      <c r="J38" s="198"/>
+      <c r="K38" s="199"/>
       <c r="M38" s="22"/>
       <c r="N38" s="22"/>
       <c r="O38" s="22"/>
@@ -10121,11 +10122,11 @@
       <c r="D39" s="33"/>
       <c r="E39" s="33"/>
       <c r="F39" s="32"/>
-      <c r="G39" s="159"/>
-      <c r="H39" s="161"/>
-      <c r="I39" s="193"/>
-      <c r="J39" s="194"/>
-      <c r="K39" s="195"/>
+      <c r="G39" s="160"/>
+      <c r="H39" s="162"/>
+      <c r="I39" s="197"/>
+      <c r="J39" s="198"/>
+      <c r="K39" s="199"/>
       <c r="M39" s="22"/>
       <c r="N39" s="22"/>
       <c r="O39" s="22"/>
@@ -10143,11 +10144,11 @@
       <c r="D40" s="33"/>
       <c r="E40" s="33"/>
       <c r="F40" s="32"/>
-      <c r="G40" s="159"/>
-      <c r="H40" s="161"/>
-      <c r="I40" s="193"/>
-      <c r="J40" s="194"/>
-      <c r="K40" s="195"/>
+      <c r="G40" s="160"/>
+      <c r="H40" s="162"/>
+      <c r="I40" s="197"/>
+      <c r="J40" s="198"/>
+      <c r="K40" s="199"/>
       <c r="M40" s="22"/>
       <c r="N40" s="22"/>
       <c r="O40" s="22"/>
@@ -10165,11 +10166,11 @@
       <c r="D41" s="33"/>
       <c r="E41" s="33"/>
       <c r="F41" s="32"/>
-      <c r="G41" s="159"/>
-      <c r="H41" s="161"/>
-      <c r="I41" s="193"/>
-      <c r="J41" s="194"/>
-      <c r="K41" s="195"/>
+      <c r="G41" s="160"/>
+      <c r="H41" s="162"/>
+      <c r="I41" s="197"/>
+      <c r="J41" s="198"/>
+      <c r="K41" s="199"/>
       <c r="M41" s="22"/>
       <c r="N41" s="22"/>
       <c r="O41" s="22"/>
@@ -10187,11 +10188,11 @@
       <c r="D42" s="33"/>
       <c r="E42" s="33"/>
       <c r="F42" s="32"/>
-      <c r="G42" s="159"/>
-      <c r="H42" s="161"/>
-      <c r="I42" s="193"/>
-      <c r="J42" s="194"/>
-      <c r="K42" s="195"/>
+      <c r="G42" s="160"/>
+      <c r="H42" s="162"/>
+      <c r="I42" s="197"/>
+      <c r="J42" s="198"/>
+      <c r="K42" s="199"/>
       <c r="M42" s="22"/>
       <c r="N42" s="22"/>
       <c r="O42" s="22"/>
@@ -10209,11 +10210,11 @@
       <c r="D43" s="33"/>
       <c r="E43" s="33"/>
       <c r="F43" s="32"/>
-      <c r="G43" s="159"/>
-      <c r="H43" s="161"/>
-      <c r="I43" s="193"/>
-      <c r="J43" s="194"/>
-      <c r="K43" s="195"/>
+      <c r="G43" s="160"/>
+      <c r="H43" s="162"/>
+      <c r="I43" s="197"/>
+      <c r="J43" s="198"/>
+      <c r="K43" s="199"/>
       <c r="M43" s="22"/>
       <c r="N43" s="22"/>
       <c r="O43" s="22"/>
@@ -10231,11 +10232,11 @@
       <c r="D44" s="33"/>
       <c r="E44" s="33"/>
       <c r="F44" s="32"/>
-      <c r="G44" s="159"/>
-      <c r="H44" s="161"/>
-      <c r="I44" s="193"/>
-      <c r="J44" s="194"/>
-      <c r="K44" s="195"/>
+      <c r="G44" s="160"/>
+      <c r="H44" s="162"/>
+      <c r="I44" s="197"/>
+      <c r="J44" s="198"/>
+      <c r="K44" s="199"/>
       <c r="M44" s="22"/>
       <c r="N44" s="22"/>
       <c r="O44" s="22"/>
@@ -10253,11 +10254,11 @@
       <c r="D45" s="33"/>
       <c r="E45" s="33"/>
       <c r="F45" s="32"/>
-      <c r="G45" s="159"/>
-      <c r="H45" s="161"/>
-      <c r="I45" s="193"/>
-      <c r="J45" s="194"/>
-      <c r="K45" s="195"/>
+      <c r="G45" s="160"/>
+      <c r="H45" s="162"/>
+      <c r="I45" s="197"/>
+      <c r="J45" s="198"/>
+      <c r="K45" s="199"/>
       <c r="M45" s="22"/>
       <c r="N45" s="22"/>
       <c r="O45" s="22"/>
@@ -10275,11 +10276,11 @@
       <c r="D46" s="33"/>
       <c r="E46" s="33"/>
       <c r="F46" s="32"/>
-      <c r="G46" s="159"/>
-      <c r="H46" s="161"/>
-      <c r="I46" s="193"/>
-      <c r="J46" s="194"/>
-      <c r="K46" s="195"/>
+      <c r="G46" s="160"/>
+      <c r="H46" s="162"/>
+      <c r="I46" s="197"/>
+      <c r="J46" s="198"/>
+      <c r="K46" s="199"/>
       <c r="M46" s="22"/>
       <c r="N46" s="22"/>
       <c r="O46" s="22"/>
@@ -10297,11 +10298,11 @@
       <c r="D47" s="33"/>
       <c r="E47" s="33"/>
       <c r="F47" s="32"/>
-      <c r="G47" s="159"/>
-      <c r="H47" s="161"/>
-      <c r="I47" s="193"/>
-      <c r="J47" s="194"/>
-      <c r="K47" s="195"/>
+      <c r="G47" s="160"/>
+      <c r="H47" s="162"/>
+      <c r="I47" s="197"/>
+      <c r="J47" s="198"/>
+      <c r="K47" s="199"/>
       <c r="M47" s="22"/>
       <c r="N47" s="22"/>
       <c r="O47" s="22"/>
@@ -10319,11 +10320,11 @@
       <c r="D48" s="33"/>
       <c r="E48" s="33"/>
       <c r="F48" s="32"/>
-      <c r="G48" s="159"/>
-      <c r="H48" s="161"/>
-      <c r="I48" s="193"/>
-      <c r="J48" s="194"/>
-      <c r="K48" s="195"/>
+      <c r="G48" s="160"/>
+      <c r="H48" s="162"/>
+      <c r="I48" s="197"/>
+      <c r="J48" s="198"/>
+      <c r="K48" s="199"/>
       <c r="M48" s="22"/>
       <c r="N48" s="22"/>
       <c r="O48" s="22"/>
@@ -10341,11 +10342,11 @@
       <c r="D49" s="33"/>
       <c r="E49" s="33"/>
       <c r="F49" s="32"/>
-      <c r="G49" s="159"/>
-      <c r="H49" s="161"/>
-      <c r="I49" s="193"/>
-      <c r="J49" s="194"/>
-      <c r="K49" s="195"/>
+      <c r="G49" s="160"/>
+      <c r="H49" s="162"/>
+      <c r="I49" s="197"/>
+      <c r="J49" s="198"/>
+      <c r="K49" s="199"/>
       <c r="M49" s="22"/>
       <c r="N49" s="22"/>
       <c r="O49" s="22"/>
@@ -10363,11 +10364,11 @@
       <c r="D50" s="33"/>
       <c r="E50" s="33"/>
       <c r="F50" s="32"/>
-      <c r="G50" s="159"/>
-      <c r="H50" s="161"/>
-      <c r="I50" s="193"/>
-      <c r="J50" s="194"/>
-      <c r="K50" s="195"/>
+      <c r="G50" s="160"/>
+      <c r="H50" s="162"/>
+      <c r="I50" s="197"/>
+      <c r="J50" s="198"/>
+      <c r="K50" s="199"/>
       <c r="M50" s="22"/>
       <c r="N50" s="22"/>
       <c r="O50" s="22"/>
@@ -10385,11 +10386,11 @@
       <c r="D51" s="33"/>
       <c r="E51" s="33"/>
       <c r="F51" s="32"/>
-      <c r="G51" s="159"/>
-      <c r="H51" s="161"/>
-      <c r="I51" s="193"/>
-      <c r="J51" s="194"/>
-      <c r="K51" s="195"/>
+      <c r="G51" s="160"/>
+      <c r="H51" s="162"/>
+      <c r="I51" s="197"/>
+      <c r="J51" s="198"/>
+      <c r="K51" s="199"/>
       <c r="M51" s="22"/>
       <c r="N51" s="22"/>
       <c r="O51" s="22"/>
@@ -10407,11 +10408,11 @@
       <c r="D52" s="33"/>
       <c r="E52" s="33"/>
       <c r="F52" s="32"/>
-      <c r="G52" s="159"/>
-      <c r="H52" s="161"/>
-      <c r="I52" s="193"/>
-      <c r="J52" s="194"/>
-      <c r="K52" s="195"/>
+      <c r="G52" s="160"/>
+      <c r="H52" s="162"/>
+      <c r="I52" s="197"/>
+      <c r="J52" s="198"/>
+      <c r="K52" s="199"/>
       <c r="M52" s="22"/>
       <c r="N52" s="22"/>
       <c r="O52" s="22"/>
@@ -10429,11 +10430,11 @@
       <c r="D53" s="33"/>
       <c r="E53" s="33"/>
       <c r="F53" s="32"/>
-      <c r="G53" s="159"/>
-      <c r="H53" s="161"/>
-      <c r="I53" s="193"/>
-      <c r="J53" s="194"/>
-      <c r="K53" s="195"/>
+      <c r="G53" s="160"/>
+      <c r="H53" s="162"/>
+      <c r="I53" s="197"/>
+      <c r="J53" s="198"/>
+      <c r="K53" s="199"/>
       <c r="M53" s="22"/>
       <c r="N53" s="22"/>
       <c r="O53" s="22"/>
@@ -10451,11 +10452,11 @@
       <c r="D54" s="33"/>
       <c r="E54" s="33"/>
       <c r="F54" s="32"/>
-      <c r="G54" s="159"/>
-      <c r="H54" s="161"/>
-      <c r="I54" s="193"/>
-      <c r="J54" s="194"/>
-      <c r="K54" s="195"/>
+      <c r="G54" s="160"/>
+      <c r="H54" s="162"/>
+      <c r="I54" s="197"/>
+      <c r="J54" s="198"/>
+      <c r="K54" s="199"/>
       <c r="M54" s="22"/>
       <c r="N54" s="22"/>
       <c r="O54" s="22"/>
@@ -10473,11 +10474,11 @@
       <c r="D55" s="33"/>
       <c r="E55" s="33"/>
       <c r="F55" s="32"/>
-      <c r="G55" s="159"/>
-      <c r="H55" s="161"/>
-      <c r="I55" s="193"/>
-      <c r="J55" s="194"/>
-      <c r="K55" s="195"/>
+      <c r="G55" s="160"/>
+      <c r="H55" s="162"/>
+      <c r="I55" s="197"/>
+      <c r="J55" s="198"/>
+      <c r="K55" s="199"/>
       <c r="M55" s="22"/>
       <c r="N55" s="22"/>
       <c r="O55" s="22"/>
@@ -10495,11 +10496,11 @@
       <c r="D56" s="33"/>
       <c r="E56" s="33"/>
       <c r="F56" s="32"/>
-      <c r="G56" s="159"/>
-      <c r="H56" s="161"/>
-      <c r="I56" s="193"/>
-      <c r="J56" s="194"/>
-      <c r="K56" s="195"/>
+      <c r="G56" s="160"/>
+      <c r="H56" s="162"/>
+      <c r="I56" s="197"/>
+      <c r="J56" s="198"/>
+      <c r="K56" s="199"/>
       <c r="M56" s="22"/>
       <c r="N56" s="22"/>
       <c r="O56" s="22"/>
@@ -10511,25 +10512,80 @@
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="107">
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="I5:K5"/>
-    <mergeCell ref="I6:K6"/>
-    <mergeCell ref="I4:K4"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="I8:K8"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="I10:K10"/>
-    <mergeCell ref="I11:K11"/>
-    <mergeCell ref="I12:K12"/>
+    <mergeCell ref="G56:H56"/>
+    <mergeCell ref="G53:H53"/>
+    <mergeCell ref="G54:H54"/>
+    <mergeCell ref="G55:H55"/>
+    <mergeCell ref="G50:H50"/>
+    <mergeCell ref="G51:H51"/>
+    <mergeCell ref="G52:H52"/>
+    <mergeCell ref="I50:K50"/>
+    <mergeCell ref="I51:K51"/>
+    <mergeCell ref="I52:K52"/>
+    <mergeCell ref="I53:K53"/>
+    <mergeCell ref="I54:K54"/>
+    <mergeCell ref="I55:K55"/>
+    <mergeCell ref="I56:K56"/>
+    <mergeCell ref="G47:H47"/>
+    <mergeCell ref="G48:H48"/>
+    <mergeCell ref="G49:H49"/>
+    <mergeCell ref="G44:H44"/>
+    <mergeCell ref="G45:H45"/>
+    <mergeCell ref="G46:H46"/>
+    <mergeCell ref="I44:K44"/>
+    <mergeCell ref="I45:K45"/>
+    <mergeCell ref="I46:K46"/>
+    <mergeCell ref="I47:K47"/>
+    <mergeCell ref="I48:K48"/>
+    <mergeCell ref="I49:K49"/>
+    <mergeCell ref="G41:H41"/>
+    <mergeCell ref="G42:H42"/>
+    <mergeCell ref="G43:H43"/>
+    <mergeCell ref="G38:H38"/>
+    <mergeCell ref="G39:H39"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="I38:K38"/>
+    <mergeCell ref="I39:K39"/>
+    <mergeCell ref="I40:K40"/>
+    <mergeCell ref="I41:K41"/>
+    <mergeCell ref="I42:K42"/>
+    <mergeCell ref="I43:K43"/>
+    <mergeCell ref="G35:H35"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="G34:H34"/>
+    <mergeCell ref="I32:K32"/>
+    <mergeCell ref="I33:K33"/>
+    <mergeCell ref="I34:K34"/>
+    <mergeCell ref="I35:K35"/>
+    <mergeCell ref="I36:K36"/>
+    <mergeCell ref="I37:K37"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="G30:H30"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="I26:K26"/>
+    <mergeCell ref="I27:K27"/>
+    <mergeCell ref="I28:K28"/>
+    <mergeCell ref="I29:K29"/>
+    <mergeCell ref="I30:K30"/>
+    <mergeCell ref="I31:K31"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="I20:K20"/>
+    <mergeCell ref="I21:K21"/>
+    <mergeCell ref="I22:K22"/>
+    <mergeCell ref="I23:K23"/>
+    <mergeCell ref="I24:K24"/>
+    <mergeCell ref="I25:K25"/>
     <mergeCell ref="G16:H16"/>
     <mergeCell ref="G17:H17"/>
     <mergeCell ref="G18:H18"/>
@@ -10544,80 +10600,25 @@
     <mergeCell ref="I17:K17"/>
     <mergeCell ref="I18:K18"/>
     <mergeCell ref="I19:K19"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="I20:K20"/>
-    <mergeCell ref="I21:K21"/>
-    <mergeCell ref="I22:K22"/>
-    <mergeCell ref="I23:K23"/>
-    <mergeCell ref="I24:K24"/>
-    <mergeCell ref="I25:K25"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="G27:H27"/>
-    <mergeCell ref="G28:H28"/>
-    <mergeCell ref="I26:K26"/>
-    <mergeCell ref="I27:K27"/>
-    <mergeCell ref="I28:K28"/>
-    <mergeCell ref="I29:K29"/>
-    <mergeCell ref="I30:K30"/>
-    <mergeCell ref="I31:K31"/>
-    <mergeCell ref="G35:H35"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="G37:H37"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="G34:H34"/>
-    <mergeCell ref="I32:K32"/>
-    <mergeCell ref="I33:K33"/>
-    <mergeCell ref="I34:K34"/>
-    <mergeCell ref="I35:K35"/>
-    <mergeCell ref="I36:K36"/>
-    <mergeCell ref="I37:K37"/>
-    <mergeCell ref="G41:H41"/>
-    <mergeCell ref="G42:H42"/>
-    <mergeCell ref="G43:H43"/>
-    <mergeCell ref="G38:H38"/>
-    <mergeCell ref="G39:H39"/>
-    <mergeCell ref="G40:H40"/>
-    <mergeCell ref="I38:K38"/>
-    <mergeCell ref="I39:K39"/>
-    <mergeCell ref="I40:K40"/>
-    <mergeCell ref="I41:K41"/>
-    <mergeCell ref="I42:K42"/>
-    <mergeCell ref="I43:K43"/>
-    <mergeCell ref="G47:H47"/>
-    <mergeCell ref="G48:H48"/>
-    <mergeCell ref="G49:H49"/>
-    <mergeCell ref="G44:H44"/>
-    <mergeCell ref="G45:H45"/>
-    <mergeCell ref="G46:H46"/>
-    <mergeCell ref="I44:K44"/>
-    <mergeCell ref="I45:K45"/>
-    <mergeCell ref="I46:K46"/>
-    <mergeCell ref="I47:K47"/>
-    <mergeCell ref="I48:K48"/>
-    <mergeCell ref="I49:K49"/>
-    <mergeCell ref="G56:H56"/>
-    <mergeCell ref="G53:H53"/>
-    <mergeCell ref="G54:H54"/>
-    <mergeCell ref="G55:H55"/>
-    <mergeCell ref="G50:H50"/>
-    <mergeCell ref="G51:H51"/>
-    <mergeCell ref="G52:H52"/>
-    <mergeCell ref="I50:K50"/>
-    <mergeCell ref="I51:K51"/>
-    <mergeCell ref="I52:K52"/>
-    <mergeCell ref="I53:K53"/>
-    <mergeCell ref="I54:K54"/>
-    <mergeCell ref="I55:K55"/>
-    <mergeCell ref="I56:K56"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="I8:K8"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="I10:K10"/>
+    <mergeCell ref="I11:K11"/>
+    <mergeCell ref="I12:K12"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="I5:K5"/>
+    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="I4:K4"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="G11:H11"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F56">
@@ -10665,16 +10666,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="25" customFormat="1" ht="12" customHeight="1">
-      <c r="A1" s="165" t="s">
+      <c r="A1" s="166" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="165"/>
-      <c r="C1" s="165"/>
-      <c r="D1" s="165"/>
-      <c r="E1" s="165"/>
-      <c r="F1" s="165"/>
-      <c r="G1" s="165"/>
-      <c r="H1" s="165"/>
+      <c r="B1" s="166"/>
+      <c r="C1" s="166"/>
+      <c r="D1" s="166"/>
+      <c r="E1" s="166"/>
+      <c r="F1" s="166"/>
+      <c r="G1" s="166"/>
+      <c r="H1" s="166"/>
       <c r="I1" s="31" t="s">
         <v>1</v>
       </c>
@@ -10709,14 +10710,14 @@
       <c r="U1" s="52"/>
     </row>
     <row r="2" spans="1:21" s="25" customFormat="1" ht="12" customHeight="1">
-      <c r="A2" s="165"/>
-      <c r="B2" s="165"/>
-      <c r="C2" s="165"/>
-      <c r="D2" s="165"/>
-      <c r="E2" s="165"/>
-      <c r="F2" s="165"/>
-      <c r="G2" s="165"/>
-      <c r="H2" s="165"/>
+      <c r="A2" s="166"/>
+      <c r="B2" s="166"/>
+      <c r="C2" s="166"/>
+      <c r="D2" s="166"/>
+      <c r="E2" s="166"/>
+      <c r="F2" s="166"/>
+      <c r="G2" s="166"/>
+      <c r="H2" s="166"/>
       <c r="I2" s="31" t="s">
         <v>2</v>
       </c>
@@ -10819,7 +10820,7 @@
       <c r="E5" s="33"/>
       <c r="F5" s="32"/>
       <c r="G5" s="88" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="H5" s="63" t="s">
         <v>185</v>
@@ -10849,7 +10850,7 @@
         <v>191</v>
       </c>
       <c r="S5" s="88" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="T5" s="64"/>
       <c r="U5" s="64"/>
@@ -10868,7 +10869,7 @@
       <c r="E6" s="33"/>
       <c r="F6" s="32"/>
       <c r="G6" s="88" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H6" s="63" t="s">
         <v>185</v>
@@ -10898,7 +10899,7 @@
         <v>191</v>
       </c>
       <c r="S6" s="88" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="T6" s="64"/>
       <c r="U6" s="64"/>
@@ -13115,11 +13116,79 @@
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="94">
-    <mergeCell ref="K88:N88"/>
-    <mergeCell ref="K89:N89"/>
-    <mergeCell ref="K90:N90"/>
-    <mergeCell ref="K91:N91"/>
-    <mergeCell ref="K92:N92"/>
+    <mergeCell ref="A1:H2"/>
+    <mergeCell ref="K14:N14"/>
+    <mergeCell ref="K15:N15"/>
+    <mergeCell ref="K16:N16"/>
+    <mergeCell ref="K17:N17"/>
+    <mergeCell ref="K12:N12"/>
+    <mergeCell ref="K13:N13"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="K4:N4"/>
+    <mergeCell ref="K7:N7"/>
+    <mergeCell ref="K8:N8"/>
+    <mergeCell ref="K9:N9"/>
+    <mergeCell ref="K10:N10"/>
+    <mergeCell ref="K11:N11"/>
+    <mergeCell ref="K18:N18"/>
+    <mergeCell ref="K19:N19"/>
+    <mergeCell ref="K20:N20"/>
+    <mergeCell ref="K21:N21"/>
+    <mergeCell ref="K22:N22"/>
+    <mergeCell ref="K23:N23"/>
+    <mergeCell ref="K24:N24"/>
+    <mergeCell ref="K25:N25"/>
+    <mergeCell ref="K26:N26"/>
+    <mergeCell ref="K27:N27"/>
+    <mergeCell ref="K28:N28"/>
+    <mergeCell ref="K29:N29"/>
+    <mergeCell ref="K30:N30"/>
+    <mergeCell ref="K31:N31"/>
+    <mergeCell ref="K32:N32"/>
+    <mergeCell ref="K33:N33"/>
+    <mergeCell ref="K34:N34"/>
+    <mergeCell ref="K35:N35"/>
+    <mergeCell ref="K36:N36"/>
+    <mergeCell ref="K37:N37"/>
+    <mergeCell ref="K38:N38"/>
+    <mergeCell ref="K39:N39"/>
+    <mergeCell ref="K40:N40"/>
+    <mergeCell ref="K41:N41"/>
+    <mergeCell ref="K58:N58"/>
+    <mergeCell ref="K53:N53"/>
+    <mergeCell ref="K59:N59"/>
+    <mergeCell ref="K42:N42"/>
+    <mergeCell ref="K43:N43"/>
+    <mergeCell ref="K44:N44"/>
+    <mergeCell ref="K45:N45"/>
+    <mergeCell ref="K46:N46"/>
+    <mergeCell ref="K47:N47"/>
+    <mergeCell ref="K48:N48"/>
+    <mergeCell ref="K49:N49"/>
+    <mergeCell ref="K50:N50"/>
+    <mergeCell ref="K54:N54"/>
+    <mergeCell ref="K55:N55"/>
+    <mergeCell ref="K56:N56"/>
+    <mergeCell ref="K57:N57"/>
+    <mergeCell ref="K51:N51"/>
+    <mergeCell ref="K52:N52"/>
+    <mergeCell ref="K93:N93"/>
+    <mergeCell ref="K94:N94"/>
+    <mergeCell ref="K5:N5"/>
+    <mergeCell ref="K6:N6"/>
+    <mergeCell ref="K78:N78"/>
+    <mergeCell ref="K79:N79"/>
+    <mergeCell ref="K80:N80"/>
+    <mergeCell ref="K81:N81"/>
+    <mergeCell ref="K82:N82"/>
+    <mergeCell ref="K83:N83"/>
+    <mergeCell ref="K84:N84"/>
+    <mergeCell ref="K85:N85"/>
+    <mergeCell ref="K86:N86"/>
+    <mergeCell ref="K69:N69"/>
+    <mergeCell ref="K70:N70"/>
+    <mergeCell ref="K71:N71"/>
     <mergeCell ref="K77:N77"/>
     <mergeCell ref="K60:N60"/>
     <mergeCell ref="K87:N87"/>
@@ -13136,79 +13205,11 @@
     <mergeCell ref="K74:N74"/>
     <mergeCell ref="K75:N75"/>
     <mergeCell ref="K76:N76"/>
-    <mergeCell ref="K93:N93"/>
-    <mergeCell ref="K94:N94"/>
-    <mergeCell ref="K5:N5"/>
-    <mergeCell ref="K6:N6"/>
-    <mergeCell ref="K78:N78"/>
-    <mergeCell ref="K79:N79"/>
-    <mergeCell ref="K80:N80"/>
-    <mergeCell ref="K81:N81"/>
-    <mergeCell ref="K82:N82"/>
-    <mergeCell ref="K83:N83"/>
-    <mergeCell ref="K84:N84"/>
-    <mergeCell ref="K85:N85"/>
-    <mergeCell ref="K86:N86"/>
-    <mergeCell ref="K69:N69"/>
-    <mergeCell ref="K70:N70"/>
-    <mergeCell ref="K71:N71"/>
-    <mergeCell ref="K59:N59"/>
-    <mergeCell ref="K42:N42"/>
-    <mergeCell ref="K43:N43"/>
-    <mergeCell ref="K44:N44"/>
-    <mergeCell ref="K45:N45"/>
-    <mergeCell ref="K46:N46"/>
-    <mergeCell ref="K47:N47"/>
-    <mergeCell ref="K48:N48"/>
-    <mergeCell ref="K49:N49"/>
-    <mergeCell ref="K50:N50"/>
-    <mergeCell ref="K54:N54"/>
-    <mergeCell ref="K55:N55"/>
-    <mergeCell ref="K56:N56"/>
-    <mergeCell ref="K57:N57"/>
-    <mergeCell ref="K51:N51"/>
-    <mergeCell ref="K52:N52"/>
-    <mergeCell ref="K38:N38"/>
-    <mergeCell ref="K39:N39"/>
-    <mergeCell ref="K40:N40"/>
-    <mergeCell ref="K41:N41"/>
-    <mergeCell ref="K58:N58"/>
-    <mergeCell ref="K53:N53"/>
-    <mergeCell ref="K33:N33"/>
-    <mergeCell ref="K34:N34"/>
-    <mergeCell ref="K35:N35"/>
-    <mergeCell ref="K36:N36"/>
-    <mergeCell ref="K37:N37"/>
-    <mergeCell ref="K28:N28"/>
-    <mergeCell ref="K29:N29"/>
-    <mergeCell ref="K30:N30"/>
-    <mergeCell ref="K31:N31"/>
-    <mergeCell ref="K32:N32"/>
-    <mergeCell ref="K23:N23"/>
-    <mergeCell ref="K24:N24"/>
-    <mergeCell ref="K25:N25"/>
-    <mergeCell ref="K26:N26"/>
-    <mergeCell ref="K27:N27"/>
-    <mergeCell ref="K18:N18"/>
-    <mergeCell ref="K19:N19"/>
-    <mergeCell ref="K20:N20"/>
-    <mergeCell ref="K21:N21"/>
-    <mergeCell ref="K22:N22"/>
-    <mergeCell ref="A1:H2"/>
-    <mergeCell ref="K14:N14"/>
-    <mergeCell ref="K15:N15"/>
-    <mergeCell ref="K16:N16"/>
-    <mergeCell ref="K17:N17"/>
-    <mergeCell ref="K12:N12"/>
-    <mergeCell ref="K13:N13"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="K4:N4"/>
-    <mergeCell ref="K7:N7"/>
-    <mergeCell ref="K8:N8"/>
-    <mergeCell ref="K9:N9"/>
-    <mergeCell ref="K10:N10"/>
-    <mergeCell ref="K11:N11"/>
+    <mergeCell ref="K88:N88"/>
+    <mergeCell ref="K89:N89"/>
+    <mergeCell ref="K90:N90"/>
+    <mergeCell ref="K91:N91"/>
+    <mergeCell ref="K92:N92"/>
   </mergeCells>
   <dataValidations count="4">
     <dataValidation allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="Q1048467:Q1048576 Q5:Q94"/>
@@ -13238,7 +13239,7 @@
   <dimension ref="A1:J87"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" customHeight="1"/>
@@ -13254,10 +13255,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="12" customHeight="1">
-      <c r="A1" s="165" t="s">
+      <c r="A1" s="166" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="165"/>
+      <c r="B1" s="166"/>
       <c r="C1" s="31" t="s">
         <v>1</v>
       </c>
@@ -13287,8 +13288,8 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="12" customHeight="1">
-      <c r="A2" s="165"/>
-      <c r="B2" s="165"/>
+      <c r="A2" s="166"/>
+      <c r="B2" s="166"/>
       <c r="C2" s="31" t="s">
         <v>2</v>
       </c>
@@ -13545,7 +13546,7 @@
     <row r="23" spans="1:10" ht="12" customHeight="1">
       <c r="B23" s="80"/>
       <c r="C23" s="43" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D23" s="43"/>
       <c r="E23" s="43"/>
@@ -14370,10 +14371,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="12" customHeight="1">
-      <c r="A1" s="165" t="s">
+      <c r="A1" s="166" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="165"/>
+      <c r="B1" s="166"/>
       <c r="C1" s="31" t="s">
         <v>1</v>
       </c>
@@ -14403,8 +14404,8 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="12" customHeight="1">
-      <c r="A2" s="165"/>
-      <c r="B2" s="165"/>
+      <c r="A2" s="166"/>
+      <c r="B2" s="166"/>
       <c r="C2" s="31" t="s">
         <v>2</v>
       </c>

</xml_diff>